<commit_message>
TA 37 Final code for review
</commit_message>
<xml_diff>
--- a/Reports/Datasheet.xlsx
+++ b/Reports/Datasheet.xlsx
@@ -8,23 +8,24 @@
   <sheets>
     <sheet name="deliveryPopulation++" r:id="rId3" sheetId="1"/>
     <sheet name="GenerateOrderSAPnumber++" r:id="rId4" sheetId="2"/>
-    <sheet name="CreateaccountBackend++" r:id="rId5" sheetId="3"/>
-    <sheet name="CheckoutpaymentOption++" r:id="rId6" sheetId="4"/>
-    <sheet name="SAP_OrderRelated++" r:id="rId7" sheetId="5"/>
-    <sheet name="PayUPagePayment++" r:id="rId8" sheetId="6"/>
-    <sheet name="OrderStatusSearch++" r:id="rId9" sheetId="7"/>
-    <sheet name="accountCreation++" r:id="rId10" sheetId="8"/>
-    <sheet name="IC" r:id="rId11" sheetId="9"/>
-    <sheet name="ic_CashDepositPayment++" r:id="rId12" sheetId="10"/>
-    <sheet name="Login_magento++" r:id="rId13" sheetId="11"/>
-    <sheet name="ProductSearch++" r:id="rId14" sheetId="12"/>
-    <sheet name="Suites" r:id="rId15" sheetId="13"/>
+    <sheet name="DB_connection_master++" r:id="rId5" sheetId="3"/>
+    <sheet name="CreateaccountBackend++" r:id="rId6" sheetId="4"/>
+    <sheet name="CheckoutpaymentOption++" r:id="rId7" sheetId="5"/>
+    <sheet name="SAP_OrderRelated++" r:id="rId8" sheetId="6"/>
+    <sheet name="PayUPagePayment++" r:id="rId9" sheetId="7"/>
+    <sheet name="OrderStatusSearch++" r:id="rId10" sheetId="8"/>
+    <sheet name="accountCreation++" r:id="rId11" sheetId="9"/>
+    <sheet name="IC" r:id="rId12" sheetId="10"/>
+    <sheet name="ic_CashDepositPayment++" r:id="rId13" sheetId="11"/>
+    <sheet name="Login_magento++" r:id="rId14" sheetId="12"/>
+    <sheet name="ProductSearch++" r:id="rId15" sheetId="13"/>
+    <sheet name="Suites" r:id="rId16" sheetId="14"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="199">
   <si>
     <t>Suburb</t>
   </si>
@@ -140,6 +141,57 @@
     <t>240</t>
   </si>
   <si>
+    <t>0005233234</t>
+  </si>
+  <si>
+    <t>DB_Instance</t>
+  </si>
+  <si>
+    <t>port</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ECCQA</t>
+  </si>
+  <si>
+    <t>30215</t>
+  </si>
+  <si>
+    <t>225505</t>
+  </si>
+  <si>
+    <t>11.19.2.172</t>
+  </si>
+  <si>
+    <t>Welc0me@2021</t>
+  </si>
+  <si>
+    <t>ECCPROD</t>
+  </si>
+  <si>
+    <t>CRMQA</t>
+  </si>
+  <si>
+    <t>1433 </t>
+  </si>
+  <si>
+    <t>cq1adm</t>
+  </si>
+  <si>
+    <t>11.19.0.68</t>
+  </si>
+  <si>
+    <t>CRMPROD</t>
+  </si>
+  <si>
     <t>Firstname</t>
   </si>
   <si>
@@ -170,7 +222,7 @@
     <t>Backend_Fisrtname</t>
   </si>
   <si>
-    <t>fake744203856514923@automationjdg.co.za</t>
+    <t>fake823493071818191@automationjdg.co.za</t>
   </si>
   <si>
     <t>11</t>
@@ -239,7 +291,7 @@
     <t>2026</t>
   </si>
   <si>
-    <t>3100000969</t>
+    <t>3100000989</t>
   </si>
   <si>
     <t>productSearchId</t>
@@ -323,7 +375,7 @@
     <t>Password2</t>
   </si>
   <si>
-    <t>fake029231624728777@automationjdg.co.za</t>
+    <t>fake181154756508120@automationjdg.co.za</t>
   </si>
   <si>
     <t>ID</t>
@@ -338,7 +390,7 @@
     <t>Create new customer in IC and Validate VAT Number</t>
   </si>
   <si>
-    <t>fake570251256341102@automationjdg.co.za</t>
+    <t>fake617702066308821@automationjdg.co.za</t>
   </si>
   <si>
     <t>Create new customer in IC and Validate ID Number</t>
@@ -347,7 +399,7 @@
     <t>4</t>
   </si>
   <si>
-    <t>fake322122237473737@automationjdg.co.za</t>
+    <t>fake484962354167058@automationjdg.co.za</t>
   </si>
   <si>
     <t>2222225</t>
@@ -359,7 +411,7 @@
     <t>5</t>
   </si>
   <si>
-    <t>fake625030886218086@automationjdg.co.za</t>
+    <t>fake340649436136746@automationjdg.co.za</t>
   </si>
   <si>
     <t>2222226</t>
@@ -371,7 +423,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>fake296064261827662@automationjdg.co.za</t>
+    <t>fake404329475182070@automationjdg.co.za</t>
   </si>
   <si>
     <t>2222227</t>
@@ -383,7 +435,7 @@
     <t>7</t>
   </si>
   <si>
-    <t>fake242679326255516@automationjdg.co.za</t>
+    <t>fake394906054750553@automationjdg.co.za</t>
   </si>
   <si>
     <t>2222228</t>
@@ -503,13 +555,10 @@
     <t>SAP_OrderRelated</t>
   </si>
   <si>
+    <t>DB_connection_master</t>
+  </si>
+  <si>
     <t>Retrived OrderID</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
   </si>
   <si>
     <t>225564</t>
@@ -876,6 +925,630 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:O13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" t="s">
+        <v>147</v>
+      </c>
+      <c r="K1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" t="s">
+        <v>149</v>
+      </c>
+      <c r="M1" t="s">
+        <v>150</v>
+      </c>
+      <c r="N1" t="s">
+        <v>151</v>
+      </c>
+      <c r="O1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J2" t="s">
+        <v>159</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>160</v>
+      </c>
+      <c r="M2" t="s">
+        <v>161</v>
+      </c>
+      <c r="N2" t="s">
+        <v>162</v>
+      </c>
+      <c r="O2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" t="s">
+        <v>165</v>
+      </c>
+      <c r="K3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" t="s">
+        <v>120</v>
+      </c>
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" t="s">
+        <v>122</v>
+      </c>
+      <c r="J5" t="s">
+        <v>122</v>
+      </c>
+      <c r="K5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>127</v>
+      </c>
+      <c r="I6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J6" t="s">
+        <v>126</v>
+      </c>
+      <c r="K6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I7" t="s">
+        <v>130</v>
+      </c>
+      <c r="J7" t="s">
+        <v>130</v>
+      </c>
+      <c r="K7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J8" t="s">
+        <v>167</v>
+      </c>
+      <c r="K8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" t="s">
+        <v>35</v>
+      </c>
+      <c r="N8" t="s">
+        <v>35</v>
+      </c>
+      <c r="O8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" t="s">
+        <v>170</v>
+      </c>
+      <c r="J9" t="s">
+        <v>171</v>
+      </c>
+      <c r="K9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N9" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D10" t="s">
+        <v>155</v>
+      </c>
+      <c r="E10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F10" t="s">
+        <v>157</v>
+      </c>
+      <c r="G10" t="s">
+        <v>172</v>
+      </c>
+      <c r="H10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" t="s">
+        <v>173</v>
+      </c>
+      <c r="J10" t="s">
+        <v>173</v>
+      </c>
+      <c r="K10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" t="s">
+        <v>162</v>
+      </c>
+      <c r="M10" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" t="s">
+        <v>174</v>
+      </c>
+      <c r="D11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E11" t="s">
+        <v>157</v>
+      </c>
+      <c r="F11" t="s">
+        <v>158</v>
+      </c>
+      <c r="G11" t="s">
+        <v>160</v>
+      </c>
+      <c r="H11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" t="s">
+        <v>75</v>
+      </c>
+      <c r="K11" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" t="s">
+        <v>161</v>
+      </c>
+      <c r="M11" t="s">
+        <v>162</v>
+      </c>
+      <c r="N11" t="s">
+        <v>175</v>
+      </c>
+      <c r="O11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" t="s">
+        <v>35</v>
+      </c>
+      <c r="O12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N13" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -887,13 +1560,13 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2">
@@ -901,7 +1574,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -915,7 +1588,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -928,13 +1601,13 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>160</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>161</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2">
@@ -942,13 +1615,13 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3">
@@ -956,13 +1629,13 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4">
@@ -970,13 +1643,13 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5">
@@ -984,13 +1657,13 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="D5" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6">
@@ -998,13 +1671,13 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="D6" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7">
@@ -1012,13 +1685,13 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C7" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="D7" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8">
@@ -1026,13 +1699,13 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9">
@@ -1040,13 +1713,13 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10">
@@ -1054,13 +1727,13 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11">
@@ -1068,13 +1741,13 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C11" t="s">
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1082,7 +1755,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1095,16 +1768,16 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="C1" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="D1" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="E1" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -1115,16 +1788,16 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="D2" t="s">
         <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="F2" t="s">
         <v>31</v>
@@ -1135,7 +1808,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -1145,45 +1818,45 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="C1" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="D1" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="E1" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="F1" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="G1" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="E2" t="s">
         <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
@@ -1191,22 +1864,22 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="E3" t="s">
         <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="G3" t="s">
         <v>25</v>
@@ -1214,22 +1887,22 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="E4" t="s">
         <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="G4" t="s">
         <v>27</v>
@@ -1237,71 +1910,71 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="E5" t="s">
         <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="G5" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="D6" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="E6" t="s">
         <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="G6" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="D7" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="E7" t="s">
         <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="G7" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1376,7 +2049,7 @@
         <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -1391,6 +2064,104 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1400,42 +2171,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="G1" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="H1" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="K1" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -1444,25 +2215,25 @@
         <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="H2" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="I2" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="J2" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="K2" t="s">
         <v>35</v>
@@ -1473,7 +2244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1486,7 +2257,7 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -1497,7 +2268,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -1508,7 +2279,7 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -1519,7 +2290,7 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -1530,7 +2301,7 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
@@ -1541,7 +2312,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -1552,9 +2323,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1565,9 +2336,12 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1576,9 +2350,12 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1587,7 +2364,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -1597,51 +2374,51 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="G2" t="s">
         <v>35</v>
@@ -1650,27 +2427,27 @@
         <v>18</v>
       </c>
       <c r="I2" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="G3" t="s">
         <v>35</v>
@@ -1679,27 +2456,27 @@
         <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="G4" t="s">
         <v>35</v>
@@ -1708,36 +2485,36 @@
         <v>27</v>
       </c>
       <c r="I4" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="G5" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="H5" t="s">
         <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1745,7 +2522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -1758,10 +2535,10 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -1772,10 +2549,10 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -1786,10 +2563,10 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
@@ -1800,10 +2577,10 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
@@ -1814,10 +2591,10 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s">
         <v>31</v>
@@ -1828,7 +2605,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:S7"/>
   <sheetViews>
@@ -1838,28 +2615,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="H1" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
@@ -1868,28 +2645,28 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="L1" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="M1" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="N1" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="O1" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="P1" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="Q1" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="R1" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="S1" t="s">
         <v>12</v>
@@ -1897,980 +2674,356 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="F2" t="s">
         <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="H2" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="I2" t="s">
         <v>18</v>
       </c>
       <c r="J2" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="K2" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="L2" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="M2" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="N2" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="O2" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="P2" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="Q2" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="R2" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="S2" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="F3" t="s">
         <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="H3" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="I3" t="s">
         <v>18</v>
       </c>
       <c r="J3" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="K3" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="L3" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="M3" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="N3" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="O3" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="P3" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="Q3" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="R3" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="S3" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="F4" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="G4" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="H4" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
       </c>
       <c r="J4" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="K4" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="L4" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="M4" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="N4" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="O4" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="P4" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="Q4" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="R4" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="S4" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="F5" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="G5" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="H5" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="I5" t="s">
         <v>18</v>
       </c>
       <c r="J5" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="K5" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="L5" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="M5" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="N5" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="O5" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="P5" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="Q5" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="R5" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="S5" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G6" t="s">
         <v>113</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
         <v>114</v>
       </c>
-      <c r="G6" t="s">
-        <v>96</v>
-      </c>
-      <c r="H6" t="s">
-        <v>93</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>97</v>
-      </c>
       <c r="K6" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="L6" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="M6" t="s">
+        <v>132</v>
+      </c>
+      <c r="N6" t="s">
         <v>115</v>
       </c>
-      <c r="N6" t="s">
-        <v>98</v>
-      </c>
       <c r="O6" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="P6" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="Q6" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="R6" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="S6" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G7" t="s">
+        <v>113</v>
+      </c>
+      <c r="H7" t="s">
+        <v>110</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>114</v>
+      </c>
+      <c r="K7" t="s">
+        <v>115</v>
+      </c>
+      <c r="L7" t="s">
+        <v>110</v>
+      </c>
+      <c r="M7" t="s">
+        <v>136</v>
+      </c>
+      <c r="N7" t="s">
+        <v>115</v>
+      </c>
+      <c r="O7" t="s">
+        <v>110</v>
+      </c>
+      <c r="P7" t="s">
         <v>117</v>
       </c>
-      <c r="F7" t="s">
+      <c r="Q7" t="s">
         <v>118</v>
       </c>
-      <c r="G7" t="s">
-        <v>96</v>
-      </c>
-      <c r="H7" t="s">
-        <v>93</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" t="s">
-        <v>97</v>
-      </c>
-      <c r="K7" t="s">
-        <v>98</v>
-      </c>
-      <c r="L7" t="s">
-        <v>93</v>
-      </c>
-      <c r="M7" t="s">
-        <v>119</v>
-      </c>
-      <c r="N7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O7" t="s">
-        <v>93</v>
-      </c>
-      <c r="P7" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>101</v>
-      </c>
       <c r="R7" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="S7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I1" t="s">
-        <v>129</v>
-      </c>
-      <c r="J1" t="s">
-        <v>130</v>
-      </c>
-      <c r="K1" t="s">
-        <v>131</v>
-      </c>
-      <c r="L1" t="s">
-        <v>132</v>
-      </c>
-      <c r="M1" t="s">
-        <v>133</v>
-      </c>
-      <c r="N1" t="s">
-        <v>134</v>
-      </c>
-      <c r="O1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" t="s">
         <v>137</v>
-      </c>
-      <c r="D2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>142</v>
-      </c>
-      <c r="J2" t="s">
-        <v>142</v>
-      </c>
-      <c r="K2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" t="s">
-        <v>143</v>
-      </c>
-      <c r="M2" t="s">
-        <v>144</v>
-      </c>
-      <c r="N2" t="s">
-        <v>145</v>
-      </c>
-      <c r="O2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>95</v>
-      </c>
-      <c r="J3" t="s">
-        <v>148</v>
-      </c>
-      <c r="K3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E4" t="s">
-        <v>149</v>
-      </c>
-      <c r="F4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" t="s">
-        <v>103</v>
-      </c>
-      <c r="J4" t="s">
-        <v>103</v>
-      </c>
-      <c r="K4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D5" t="s">
-        <v>143</v>
-      </c>
-      <c r="E5" t="s">
-        <v>149</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" t="s">
-        <v>106</v>
-      </c>
-      <c r="I5" t="s">
-        <v>105</v>
-      </c>
-      <c r="J5" t="s">
-        <v>105</v>
-      </c>
-      <c r="K5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" t="s">
-        <v>137</v>
-      </c>
-      <c r="D6" t="s">
-        <v>143</v>
-      </c>
-      <c r="E6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" t="s">
-        <v>110</v>
-      </c>
-      <c r="I6" t="s">
-        <v>109</v>
-      </c>
-      <c r="J6" t="s">
-        <v>109</v>
-      </c>
-      <c r="K6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D7" t="s">
-        <v>143</v>
-      </c>
-      <c r="E7" t="s">
-        <v>149</v>
-      </c>
-      <c r="F7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" t="s">
-        <v>114</v>
-      </c>
-      <c r="I7" t="s">
-        <v>113</v>
-      </c>
-      <c r="J7" t="s">
-        <v>113</v>
-      </c>
-      <c r="K7" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" t="s">
-        <v>35</v>
-      </c>
-      <c r="N7" t="s">
-        <v>35</v>
-      </c>
-      <c r="O7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C8" t="s">
-        <v>137</v>
-      </c>
-      <c r="D8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" t="s">
-        <v>118</v>
-      </c>
-      <c r="I8" t="s">
-        <v>150</v>
-      </c>
-      <c r="J8" t="s">
-        <v>150</v>
-      </c>
-      <c r="K8" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" t="s">
-        <v>35</v>
-      </c>
-      <c r="N8" t="s">
-        <v>35</v>
-      </c>
-      <c r="O8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>151</v>
-      </c>
-      <c r="B9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C9" t="s">
-        <v>137</v>
-      </c>
-      <c r="D9" t="s">
-        <v>152</v>
-      </c>
-      <c r="E9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9" t="s">
-        <v>153</v>
-      </c>
-      <c r="J9" t="s">
-        <v>154</v>
-      </c>
-      <c r="K9" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" t="s">
-        <v>35</v>
-      </c>
-      <c r="M9" t="s">
-        <v>35</v>
-      </c>
-      <c r="N9" t="s">
-        <v>35</v>
-      </c>
-      <c r="O9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>151</v>
-      </c>
-      <c r="B10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C10" t="s">
-        <v>137</v>
-      </c>
-      <c r="D10" t="s">
-        <v>138</v>
-      </c>
-      <c r="E10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F10" t="s">
-        <v>140</v>
-      </c>
-      <c r="G10" t="s">
-        <v>155</v>
-      </c>
-      <c r="H10" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" t="s">
-        <v>156</v>
-      </c>
-      <c r="J10" t="s">
-        <v>156</v>
-      </c>
-      <c r="K10" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" t="s">
-        <v>145</v>
-      </c>
-      <c r="M10" t="s">
-        <v>35</v>
-      </c>
-      <c r="N10" t="s">
-        <v>35</v>
-      </c>
-      <c r="O10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>151</v>
-      </c>
-      <c r="B11" t="s">
-        <v>136</v>
-      </c>
-      <c r="C11" t="s">
-        <v>157</v>
-      </c>
-      <c r="D11" t="s">
-        <v>139</v>
-      </c>
-      <c r="E11" t="s">
-        <v>140</v>
-      </c>
-      <c r="F11" t="s">
-        <v>141</v>
-      </c>
-      <c r="G11" t="s">
-        <v>143</v>
-      </c>
-      <c r="H11" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" t="s">
-        <v>58</v>
-      </c>
-      <c r="J11" t="s">
-        <v>58</v>
-      </c>
-      <c r="K11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L11" t="s">
-        <v>144</v>
-      </c>
-      <c r="M11" t="s">
-        <v>145</v>
-      </c>
-      <c r="N11" t="s">
-        <v>158</v>
-      </c>
-      <c r="O11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J12" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12" t="s">
-        <v>35</v>
-      </c>
-      <c r="L12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M12" t="s">
-        <v>35</v>
-      </c>
-      <c r="N12" t="s">
-        <v>35</v>
-      </c>
-      <c r="O12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" t="s">
-        <v>35</v>
-      </c>
-      <c r="L13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M13" t="s">
-        <v>35</v>
-      </c>
-      <c r="N13" t="s">
-        <v>35</v>
-      </c>
-      <c r="O13" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
main update end to end
</commit_message>
<xml_diff>
--- a/Reports/Datasheet.xlsx
+++ b/Reports/Datasheet.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="235">
   <si>
     <t>Suburb</t>
   </si>
@@ -118,6 +118,12 @@
     <t>9</t>
   </si>
   <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>AutoJDGTest@gmail.com</t>
+  </si>
+  <si>
     <t>totalCounter</t>
   </si>
   <si>
@@ -154,12 +160,6 @@
     <t>Password@123</t>
   </si>
   <si>
-    <t>AutoJDGTest@gmail.com</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
     <t>Password2</t>
   </si>
   <si>
@@ -193,7 +193,7 @@
     <t>Backend_Fisrtname</t>
   </si>
   <si>
-    <t>fake488867862021878@automationjdg.co.za</t>
+    <t>fake223146100024430@automationjdg.co.za</t>
   </si>
   <si>
     <t>11</t>
@@ -331,7 +331,7 @@
     <t>Brian</t>
   </si>
   <si>
-    <t>fake787275058514350@automationjdg.co.za</t>
+    <t>fake430243281580300@automationjdg.co.za</t>
   </si>
   <si>
     <t>ID</t>
@@ -346,7 +346,7 @@
     <t>Create new customer in IC and Validate VAT Number</t>
   </si>
   <si>
-    <t>fake360456087699750@automationjdg.co.za</t>
+    <t>fake405166777548214@automationjdg.co.za</t>
   </si>
   <si>
     <t>Create new customer in IC and Validate ID Number</t>
@@ -364,7 +364,7 @@
     <t>5</t>
   </si>
   <si>
-    <t>fake649617047845586@automationjdg.co.za</t>
+    <t>fake736557570573372@automationjdg.co.za</t>
   </si>
   <si>
     <t>2222226</t>
@@ -376,7 +376,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>fake727956141588867@automationjdg.co.za</t>
+    <t>fake407521424325957@automationjdg.co.za</t>
   </si>
   <si>
     <t>2222227</t>
@@ -388,7 +388,7 @@
     <t>7</t>
   </si>
   <si>
-    <t>fake587267550208061@automationjdg.co.za</t>
+    <t>fake185322043795860@automationjdg.co.za</t>
   </si>
   <si>
     <t>2222228</t>
@@ -517,12 +517,12 @@
     <t>yes</t>
   </si>
   <si>
+    <t>Gift card purchase verifiacation Sender</t>
+  </si>
+  <si>
     <t>icGiftCardVerificationSender</t>
   </si>
   <si>
-    <t>Gift card purchase verifiacation Sender</t>
-  </si>
-  <si>
     <t>Test Case name</t>
   </si>
   <si>
@@ -557,9 +557,6 @@
   </si>
   <si>
     <t>Rashad</t>
-  </si>
-  <si>
-    <t>AutoJDGTest2@gmail.com</t>
   </si>
   <si>
     <t>Kelly</t>
@@ -778,7 +775,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -986,6 +983,47 @@
         <v>23</v>
       </c>
       <c r="M5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1027,7 +1065,7 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1037,7 +1075,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1086,25 +1124,57 @@
         <v>176</v>
       </c>
       <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
         <v>177</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>178</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
         <v>179</v>
       </c>
-      <c r="G2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" t="s">
-        <v>180</v>
-      </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>179</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1125,13 +1195,13 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2">
@@ -1139,13 +1209,13 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>181</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="3">
@@ -1153,13 +1223,13 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4">
@@ -1167,13 +1237,13 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5">
@@ -1181,13 +1251,13 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C5" t="s">
         <v>108</v>
       </c>
       <c r="D5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6">
@@ -1195,13 +1265,13 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C6" t="s">
         <v>111</v>
       </c>
       <c r="D6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7">
@@ -1209,13 +1279,13 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C7" t="s">
         <v>115</v>
       </c>
       <c r="D7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8">
@@ -1223,13 +1293,13 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C8" t="s">
         <v>119</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9">
@@ -1237,13 +1307,13 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C9" t="s">
         <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10">
@@ -1251,13 +1321,13 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11">
@@ -1265,13 +1335,13 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
+        <v>180</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
         <v>181</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1292,16 +1362,16 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" t="s">
         <v>183</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>184</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>185</v>
-      </c>
-      <c r="E1" t="s">
-        <v>186</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -1312,7 +1382,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C2" t="s">
         <v>115</v>
@@ -1321,7 +1391,7 @@
         <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F2" t="s">
         <v>18</v>
@@ -1332,7 +1402,7 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C3" t="s">
         <v>115</v>
@@ -1341,7 +1411,7 @@
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F3" t="s">
         <v>25</v>
@@ -1352,16 +1422,16 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
         <v>189</v>
       </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>190</v>
-      </c>
-      <c r="E4" t="s">
-        <v>191</v>
       </c>
       <c r="F4" t="s">
         <v>27</v>
@@ -1372,16 +1442,16 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
         <v>192</v>
       </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>193</v>
-      </c>
-      <c r="E5" t="s">
-        <v>194</v>
       </c>
       <c r="F5" t="s">
         <v>111</v>
@@ -1392,16 +1462,16 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
         <v>195</v>
       </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>196</v>
-      </c>
-      <c r="E6" t="s">
-        <v>197</v>
       </c>
       <c r="F6" t="s">
         <v>115</v>
@@ -1412,16 +1482,16 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F7" t="s">
         <v>119</v>
@@ -1432,16 +1502,16 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
         <v>59</v>
@@ -1452,16 +1522,16 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
         <v>29</v>
@@ -1472,19 +1542,19 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11">
@@ -1492,16 +1562,16 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F11" t="s">
         <v>56</v>
@@ -1512,19 +1582,19 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
+        <v>202</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
         <v>203</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="13">
@@ -1532,19 +1602,19 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
         <v>205</v>
-      </c>
-      <c r="C13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="14">
@@ -1552,19 +1622,19 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
+        <v>206</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
         <v>207</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="15">
@@ -1572,19 +1642,19 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16">
@@ -1592,19 +1662,19 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F16" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17">
@@ -1612,19 +1682,19 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
         <v>211</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="18">
@@ -1632,19 +1702,19 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
+        <v>212</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" t="s">
         <v>213</v>
-      </c>
-      <c r="C18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" t="s">
-        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -1668,31 +1738,31 @@
         <v>90</v>
       </c>
       <c r="C1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" t="s">
         <v>215</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>216</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>217</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>218</v>
-      </c>
-      <c r="G1" t="s">
-        <v>219</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1" t="s">
         <v>220</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>221</v>
-      </c>
-      <c r="K1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="2">
@@ -1700,34 +1770,34 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K2" t="s">
-        <v>108</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1745,30 +1815,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B1" t="s">
         <v>124</v>
       </c>
       <c r="C1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" t="s">
         <v>225</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>226</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>227</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>228</v>
-      </c>
-      <c r="G1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B2" t="s">
         <v>162</v>
@@ -1780,7 +1850,7 @@
         <v>138</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
         <v>138</v>
@@ -1791,7 +1861,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B3" t="s">
         <v>138</v>
@@ -1803,7 +1873,7 @@
         <v>138</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
         <v>138</v>
@@ -1814,7 +1884,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B4" t="s">
         <v>138</v>
@@ -1826,7 +1896,7 @@
         <v>138</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
         <v>138</v>
@@ -1837,7 +1907,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B5" t="s">
         <v>138</v>
@@ -1849,7 +1919,7 @@
         <v>138</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
         <v>138</v>
@@ -1860,7 +1930,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B6" t="s">
         <v>138</v>
@@ -1872,7 +1942,7 @@
         <v>138</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
         <v>138</v>
@@ -1883,7 +1953,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B7" t="s">
         <v>138</v>
@@ -1895,7 +1965,7 @@
         <v>138</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
         <v>138</v>
@@ -1922,16 +1992,16 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2">
@@ -1939,16 +2009,16 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3">
@@ -1956,16 +2026,16 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4">
@@ -1973,16 +2043,16 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2003,13 +2073,13 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2">
@@ -2017,13 +2087,13 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3">
@@ -2031,10 +2101,10 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>44</v>
@@ -2096,7 +2166,7 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>55</v>
@@ -2120,7 +2190,7 @@
         <v>60</v>
       </c>
       <c r="K2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2130,7 +2200,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2199,7 +2269,18 @@
         <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2209,7 +2290,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2264,7 +2345,7 @@
         <v>74</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
         <v>18</v>
@@ -2293,7 +2374,7 @@
         <v>74</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
         <v>25</v>
@@ -2322,7 +2403,7 @@
         <v>74</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
         <v>27</v>
@@ -2351,12 +2432,41 @@
         <v>74</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2440,7 +2550,7 @@
         <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2671,7 +2781,7 @@
         <v>96</v>
       </c>
       <c r="M4" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="N4" t="s">
         <v>44</v>
@@ -2931,7 +3041,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>137</v>
@@ -2961,7 +3071,7 @@
         <v>143</v>
       </c>
       <c r="K2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L2" t="s">
         <v>144</v>
@@ -2973,12 +3083,12 @@
         <v>146</v>
       </c>
       <c r="O2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
         <v>147</v>
@@ -2990,13 +3100,13 @@
         <v>148</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
         <v>25</v>
@@ -3008,24 +3118,24 @@
         <v>149</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
         <v>147</v>
@@ -3040,10 +3150,10 @@
         <v>150</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
         <v>27</v>
@@ -3055,24 +3165,24 @@
         <v>105</v>
       </c>
       <c r="K4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
         <v>147</v>
@@ -3087,10 +3197,10 @@
         <v>150</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H5" t="s">
         <v>108</v>
@@ -3102,24 +3212,24 @@
         <v>107</v>
       </c>
       <c r="K5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
         <v>147</v>
@@ -3134,10 +3244,10 @@
         <v>150</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
         <v>111</v>
@@ -3149,24 +3259,24 @@
         <v>110</v>
       </c>
       <c r="K6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>147</v>
@@ -3181,10 +3291,10 @@
         <v>150</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H7" t="s">
         <v>115</v>
@@ -3196,24 +3306,24 @@
         <v>114</v>
       </c>
       <c r="K7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
         <v>147</v>
@@ -3228,10 +3338,10 @@
         <v>150</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H8" t="s">
         <v>119</v>
@@ -3243,19 +3353,19 @@
         <v>151</v>
       </c>
       <c r="K8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9">
@@ -3272,13 +3382,13 @@
         <v>153</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H9" t="s">
         <v>59</v>
@@ -3290,19 +3400,19 @@
         <v>155</v>
       </c>
       <c r="K9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10">
@@ -3337,24 +3447,24 @@
         <v>157</v>
       </c>
       <c r="K10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L10" t="s">
         <v>146</v>
       </c>
       <c r="M10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>158</v>
@@ -3375,7 +3485,7 @@
         <v>144</v>
       </c>
       <c r="H11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I11" t="s">
         <v>160</v>
@@ -3384,7 +3494,7 @@
         <v>160</v>
       </c>
       <c r="K11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L11" t="s">
         <v>145</v>
@@ -3393,15 +3503,15 @@
         <v>146</v>
       </c>
       <c r="N11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
         <v>161</v>
@@ -3410,40 +3520,40 @@
         <v>162</v>
       </c>
       <c r="D12" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" t="s">
+        <v>159</v>
+      </c>
+      <c r="F12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G12" t="s">
+        <v>156</v>
+      </c>
+      <c r="H12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" t="s">
         <v>163</v>
       </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
+        <v>163</v>
+      </c>
+      <c r="K12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" t="s">
         <v>164</v>
       </c>
-      <c r="J12" t="s">
-        <v>164</v>
-      </c>
-      <c r="K12" t="s">
-        <v>34</v>
-      </c>
-      <c r="L12" t="s">
-        <v>34</v>
-      </c>
       <c r="M12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Search Bar - Minimum Character
</commit_message>
<xml_diff>
--- a/Reports/Datasheet.xlsx
+++ b/Reports/Datasheet.xlsx
@@ -867,7 +867,7 @@
     <t>Backend_Lastname</t>
   </si>
   <si>
-    <t>fake405037554824917@automationjdg.co.za</t>
+    <t>fake107526867660112@automationjdg.co.za</t>
   </si>
   <si>
     <t>7503226018089</t>
@@ -876,10 +876,10 @@
     <t>Main Website</t>
   </si>
   <si>
-    <t>fake515576077547784@automationjdg.co.za</t>
-  </si>
-  <si>
-    <t>fake055933214637283@automationjdg.co.za</t>
+    <t>fake261611228615313@automationjdg.co.za</t>
+  </si>
+  <si>
+    <t>fake164096487844381@automationjdg.co.za</t>
   </si>
   <si>
     <t>abcd1234</t>
@@ -930,7 +930,7 @@
     <t>Jones</t>
   </si>
   <si>
-    <t>fake883903505047606@automationjdg.co.za</t>
+    <t>fake041558779642091@automationjdg.co.za</t>
   </si>
   <si>
     <t>2222224</t>
@@ -945,7 +945,7 @@
     <t>5311266534086</t>
   </si>
   <si>
-    <t>fake827514183850000@automationjdg.co.za</t>
+    <t>fake634140485849656@automationjdg.co.za</t>
   </si>
   <si>
     <t>9708027466084</t>
@@ -957,13 +957,13 @@
     <t>5311ABGF25</t>
   </si>
   <si>
-    <t>fake488984763711713@automationjdg.co.za</t>
+    <t>fake501709322618150@automationjdg.co.za</t>
   </si>
   <si>
     <t>2222226</t>
   </si>
   <si>
-    <t>fake940066830044150@automationjdg.co.za</t>
+    <t>fake581920703738205@automationjdg.co.za</t>
   </si>
   <si>
     <t>2222227</t>
@@ -975,7 +975,7 @@
     <t>Create New Customer - Validate Registration Form - validate Existing Account</t>
   </si>
   <si>
-    <t>fake585408232110480@automationjdg.co.za</t>
+    <t>fake616337510515276@automationjdg.co.za</t>
   </si>
   <si>
     <t>22</t>
@@ -984,7 +984,7 @@
     <t>Create New Customer - Validate Registration Form -Password Field</t>
   </si>
   <si>
-    <t>fake218396824073864@automationjdg.co.za</t>
+    <t>fake938294267416205@automationjdg.co.za</t>
   </si>
   <si>
     <t>23</t>
@@ -993,7 +993,7 @@
     <t>Create New Customer - Validate Registration Form - SAID Field With Less than 13 Digits</t>
   </si>
   <si>
-    <t>fake418388269301706@automationjdg.co.za</t>
+    <t>fake434879418133034@automationjdg.co.za</t>
   </si>
   <si>
     <t>24</t>
@@ -1002,7 +1002,7 @@
     <t>Create New Customer - Validate Registration Form -- SAID Field With More than 13 Digits</t>
   </si>
   <si>
-    <t>fake474057028134402@automationjdg.co.za</t>
+    <t>fake702326010663179@automationjdg.co.za</t>
   </si>
   <si>
     <t>25</t>
@@ -1011,7 +1011,7 @@
     <t>Create New Customer - Validate Registration Form - Incorrect SAID</t>
   </si>
   <si>
-    <t>fake911207664109317@automationjdg.co.za</t>
+    <t>fake917642106090980@automationjdg.co.za</t>
   </si>
   <si>
     <t>TestCaseID</t>

</xml_diff>

<commit_message>
End to End run completed
</commit_message>
<xml_diff>
--- a/Reports/Datasheet.xlsx
+++ b/Reports/Datasheet.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="285">
   <si>
     <t>testSuitID</t>
   </si>
@@ -276,6 +276,15 @@
   </si>
   <si>
     <t>icLogoHomepage</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>Verify popular search in IC</t>
+  </si>
+  <si>
+    <t>icPopularSearch</t>
   </si>
   <si>
     <t>TCID</t>
@@ -1108,16 +1117,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2">
@@ -1149,13 +1158,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2">
@@ -1166,7 +1175,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3">
@@ -1177,7 +1186,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4">
@@ -1188,7 +1197,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5">
@@ -1199,7 +1208,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6">
@@ -1210,18 +1219,18 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1239,37 +1248,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="G1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="H1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="I1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="J1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="K1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2">
@@ -1280,28 +1289,28 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="F2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="G2" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="J2" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="K2" t="s">
         <v>11</v>
@@ -1322,61 +1331,61 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="G1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="H1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="I1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="J1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="K1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="L1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="M1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="N1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="O1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="P1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="Q1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="R1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="S1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2">
@@ -1390,52 +1399,52 @@
         <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="J2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="K2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="L2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="M2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="N2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="O2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="P2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="Q2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="R2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="S2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3">
@@ -1449,52 +1458,52 @@
         <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F3" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="J3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="K3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="L3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="M3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="N3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="O3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="P3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="Q3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="R3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="S3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4">
@@ -1508,52 +1517,52 @@
         <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I4" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="J4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K4" t="s">
+        <v>187</v>
+      </c>
+      <c r="L4" t="s">
+        <v>143</v>
+      </c>
+      <c r="M4" t="s">
         <v>188</v>
       </c>
-      <c r="K4" t="s">
-        <v>184</v>
-      </c>
-      <c r="L4" t="s">
-        <v>140</v>
-      </c>
-      <c r="M4" t="s">
-        <v>185</v>
-      </c>
       <c r="N4" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="O4" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="P4" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="Q4" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="R4" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="S4" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5">
@@ -1567,52 +1576,52 @@
         <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E5" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F5" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G5" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H5" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="J5" t="s">
+        <v>192</v>
+      </c>
+      <c r="K5" t="s">
+        <v>187</v>
+      </c>
+      <c r="L5" t="s">
+        <v>143</v>
+      </c>
+      <c r="M5" t="s">
+        <v>158</v>
+      </c>
+      <c r="N5" t="s">
         <v>189</v>
       </c>
-      <c r="K5" t="s">
-        <v>184</v>
-      </c>
-      <c r="L5" t="s">
-        <v>140</v>
-      </c>
-      <c r="M5" t="s">
-        <v>155</v>
-      </c>
-      <c r="N5" t="s">
-        <v>186</v>
-      </c>
       <c r="O5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="P5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="Q5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="R5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="S5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6">
@@ -1626,52 +1635,52 @@
         <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E6" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F6" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G6" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H6" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I6" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="J6" t="s">
+        <v>193</v>
+      </c>
+      <c r="K6" t="s">
+        <v>187</v>
+      </c>
+      <c r="L6" t="s">
         <v>190</v>
       </c>
-      <c r="K6" t="s">
-        <v>184</v>
-      </c>
-      <c r="L6" t="s">
-        <v>187</v>
-      </c>
       <c r="M6" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="N6" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="O6" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="P6" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="Q6" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="R6" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="S6" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7">
@@ -1682,55 +1691,55 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D7" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E7" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F7" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G7" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H7" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="J7" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="K7" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="L7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="M7" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="N7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="O7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="P7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="Q7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="R7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="S7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1748,16 +1757,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2">
@@ -1768,10 +1777,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3">
@@ -1782,10 +1791,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4">
@@ -1796,10 +1805,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5">
@@ -1810,10 +1819,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D5" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6">
@@ -1824,10 +1833,10 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D6" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7">
@@ -1838,10 +1847,10 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D7" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8">
@@ -1852,10 +1861,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D8" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9">
@@ -1866,10 +1875,10 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D9" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10">
@@ -1880,10 +1889,10 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11">
@@ -1894,10 +1903,10 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D11" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -1915,19 +1924,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2">
@@ -1938,10 +1947,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -1955,10 +1964,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -1972,10 +1981,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -1996,16 +2005,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2">
@@ -2016,10 +2025,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3">
@@ -2030,10 +2039,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4">
@@ -2044,10 +2053,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D4" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5">
@@ -2058,10 +2067,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2079,22 +2088,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2">
@@ -2105,10 +2114,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -2125,10 +2134,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D3" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -2145,13 +2154,13 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D4" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E4" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
@@ -2165,13 +2174,13 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D5" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E5" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
@@ -2185,13 +2194,13 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D6" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E6" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
@@ -2205,10 +2214,10 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D7" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -2225,10 +2234,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D8" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -2245,10 +2254,10 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D9" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -2259,16 +2268,16 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D10" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
@@ -2279,16 +2288,16 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D11" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -2299,16 +2308,16 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D12" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -2319,16 +2328,16 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D13" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -2339,16 +2348,16 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D14" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -2365,10 +2374,10 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D15" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -2379,16 +2388,16 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D16" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -2405,10 +2414,10 @@
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D17" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
@@ -2425,10 +2434,10 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D18" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -2455,7 +2464,7 @@
         <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
@@ -2496,25 +2505,25 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F2" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="G2" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
@@ -2540,22 +2549,22 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F3" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -2597,43 +2606,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="F1" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="G1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="H1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="I1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="J1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="K1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="L1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="M1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2">
@@ -2644,37 +2653,37 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D2" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E2" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F2" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="G2" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="H2" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="I2" t="s">
+        <v>257</v>
+      </c>
+      <c r="J2" t="s">
+        <v>258</v>
+      </c>
+      <c r="K2" t="s">
         <v>254</v>
       </c>
-      <c r="J2" t="s">
-        <v>255</v>
-      </c>
-      <c r="K2" t="s">
-        <v>251</v>
-      </c>
       <c r="L2" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="M2" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3">
@@ -2685,37 +2694,37 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D3" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E3" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F3" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="G3" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="H3" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="I3" t="s">
+        <v>257</v>
+      </c>
+      <c r="J3" t="s">
+        <v>258</v>
+      </c>
+      <c r="K3" t="s">
         <v>254</v>
       </c>
-      <c r="J3" t="s">
-        <v>255</v>
-      </c>
-      <c r="K3" t="s">
-        <v>251</v>
-      </c>
       <c r="L3" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="M3" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4">
@@ -2726,37 +2735,37 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D4" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E4" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F4" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="G4" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="H4" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="I4" t="s">
+        <v>257</v>
+      </c>
+      <c r="J4" t="s">
+        <v>258</v>
+      </c>
+      <c r="K4" t="s">
         <v>254</v>
       </c>
-      <c r="J4" t="s">
-        <v>255</v>
-      </c>
-      <c r="K4" t="s">
-        <v>251</v>
-      </c>
       <c r="L4" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="M4" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5">
@@ -2767,78 +2776,78 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E5" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="G5" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="H5" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="I5" t="s">
+        <v>257</v>
+      </c>
+      <c r="J5" t="s">
+        <v>258</v>
+      </c>
+      <c r="K5" t="s">
         <v>254</v>
       </c>
-      <c r="J5" t="s">
-        <v>255</v>
-      </c>
-      <c r="K5" t="s">
-        <v>251</v>
-      </c>
       <c r="L5" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="M5" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D6" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E6" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F6" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="G6" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="H6" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="I6" t="s">
+        <v>257</v>
+      </c>
+      <c r="J6" t="s">
+        <v>258</v>
+      </c>
+      <c r="K6" t="s">
         <v>254</v>
       </c>
-      <c r="J6" t="s">
-        <v>255</v>
-      </c>
-      <c r="K6" t="s">
-        <v>251</v>
-      </c>
       <c r="L6" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="M6" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2848,7 +2857,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3476,7 +3485,7 @@
         <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
         <v>71</v>
@@ -3509,6 +3518,53 @@
         <v>11</v>
       </c>
       <c r="O14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" t="s">
+        <v>11</v>
+      </c>
+      <c r="N15" t="s">
+        <v>11</v>
+      </c>
+      <c r="O15" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3527,16 +3583,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2">
@@ -3547,10 +3603,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D2" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3">
@@ -3561,10 +3617,10 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D3" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4">
@@ -3575,10 +3631,10 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D4" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5">
@@ -3589,10 +3645,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D5" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6">
@@ -3603,10 +3659,10 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D6" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7">
@@ -3617,10 +3673,10 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D7" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8">
@@ -3631,10 +3687,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D8" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9">
@@ -3645,10 +3701,10 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D9" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10">
@@ -3659,10 +3715,10 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D10" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11">
@@ -3673,10 +3729,10 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D11" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12">
@@ -3687,10 +3743,10 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D12" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13">
@@ -3701,10 +3757,10 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D13" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -3722,31 +3778,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="E1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="F1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="G1" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="H1" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="I1" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2">
@@ -3757,22 +3813,22 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D2" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="E2" t="s">
         <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G2" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="H2" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
@@ -3786,22 +3842,22 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D3" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="E3" t="s">
         <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G3" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="H3" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
@@ -3815,22 +3871,22 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D4" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="E4" t="s">
         <v>57</v>
       </c>
       <c r="F4" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G4" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="H4" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="I4" t="s">
         <v>11</v>
@@ -3844,22 +3900,22 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D5" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="E5" t="s">
         <v>57</v>
       </c>
       <c r="F5" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G5" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="H5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="I5" t="s">
         <v>11</v>
@@ -3867,28 +3923,28 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D6" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="E6" t="s">
         <v>57</v>
       </c>
       <c r="F6" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G6" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="H6" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="I6" t="s">
         <v>11</v>
@@ -3953,19 +4009,19 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E2" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F2" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -3994,19 +4050,19 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E3" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F3" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -4089,19 +4145,19 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E2" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F2" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -4130,19 +4186,19 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E3" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F3" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -4225,19 +4281,19 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E2" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F2" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -4266,19 +4322,19 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E3" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F3" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -4361,19 +4417,19 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E2" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F2" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -4402,19 +4458,19 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E3" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F3" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -4453,30 +4509,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3">
@@ -4487,10 +4543,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -4508,42 +4564,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3">
@@ -4554,16 +4610,16 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -4581,16 +4637,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2">
@@ -4601,24 +4657,24 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4">
@@ -4629,10 +4685,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5">
@@ -4643,10 +4699,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -4664,16 +4720,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2">
@@ -4684,24 +4740,24 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -4719,22 +4775,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G1" t="s">
         <v>11</v>
@@ -4742,22 +4798,22 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -4765,7 +4821,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -4788,22 +4844,22 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E4" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F4" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -4811,7 +4867,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -4847,37 +4903,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="I1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="J1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="K1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2">
@@ -4888,10 +4944,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -4903,7 +4959,7 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
@@ -4917,16 +4973,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -4938,7 +4994,7 @@
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
@@ -4965,34 +5021,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="I1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="J1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
@@ -5003,60 +5059,60 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="G2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="I2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="J2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="G3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="I3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="J3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enter invalid email address
</commit_message>
<xml_diff>
--- a/Reports/Datasheet.xlsx
+++ b/Reports/Datasheet.xlsx
@@ -12,35 +12,36 @@
     <sheet name="SapCustomer++" r:id="rId6" sheetId="4"/>
     <sheet name="Suites" r:id="rId7" sheetId="5"/>
     <sheet name="PayUPagePayment++" r:id="rId8" sheetId="6"/>
-    <sheet name="CheckoutpaymentOption++" r:id="rId9" sheetId="7"/>
-    <sheet name="deliveryPopulation++" r:id="rId10" sheetId="8"/>
-    <sheet name="icGiftCardPurchase++" r:id="rId11" sheetId="9"/>
-    <sheet name="SAP_OrderRelated++" r:id="rId12" sheetId="10"/>
-    <sheet name="GenerateOrderSAPnumber++" r:id="rId13" sheetId="11"/>
-    <sheet name="OrderStatusSearch++" r:id="rId14" sheetId="12"/>
-    <sheet name="Login_magento++" r:id="rId15" sheetId="13"/>
-    <sheet name="ic_RetriveOrderID++" r:id="rId16" sheetId="14"/>
-    <sheet name="ProductSearch++" r:id="rId17" sheetId="15"/>
-    <sheet name="icRedeemGiftCard++" r:id="rId18" sheetId="16"/>
-    <sheet name="VeriyGiftcardUsableity++" r:id="rId19" sheetId="17"/>
-    <sheet name="ic_login++" r:id="rId20" sheetId="18"/>
-    <sheet name="DB_connection_master++" r:id="rId21" sheetId="19"/>
-    <sheet name="icGiftCardVerificationSender++" r:id="rId22" sheetId="20"/>
-    <sheet name="ic_CashDepositPayment++" r:id="rId23" sheetId="21"/>
-    <sheet name="CreateaccountBackend++" r:id="rId24" sheetId="22"/>
-    <sheet name="accountCreation++" r:id="rId25" sheetId="23"/>
-    <sheet name="Russels" r:id="rId26" sheetId="24"/>
-    <sheet name="Login++" r:id="rId27" sheetId="25"/>
-    <sheet name="Bradlows" r:id="rId28" sheetId="26"/>
-    <sheet name="Rochester" r:id="rId29" sheetId="27"/>
-    <sheet name="Sleepmasters" r:id="rId30" sheetId="28"/>
-    <sheet name="HiFiCorp" r:id="rId31" sheetId="29"/>
+    <sheet name="icInvalidEmail++" r:id="rId9" sheetId="7"/>
+    <sheet name="CheckoutpaymentOption++" r:id="rId10" sheetId="8"/>
+    <sheet name="deliveryPopulation++" r:id="rId11" sheetId="9"/>
+    <sheet name="icGiftCardPurchase++" r:id="rId12" sheetId="10"/>
+    <sheet name="SAP_OrderRelated++" r:id="rId13" sheetId="11"/>
+    <sheet name="GenerateOrderSAPnumber++" r:id="rId14" sheetId="12"/>
+    <sheet name="OrderStatusSearch++" r:id="rId15" sheetId="13"/>
+    <sheet name="Login_magento++" r:id="rId16" sheetId="14"/>
+    <sheet name="ic_RetriveOrderID++" r:id="rId17" sheetId="15"/>
+    <sheet name="ProductSearch++" r:id="rId18" sheetId="16"/>
+    <sheet name="icRedeemGiftCard++" r:id="rId19" sheetId="17"/>
+    <sheet name="VeriyGiftcardUsableity++" r:id="rId20" sheetId="18"/>
+    <sheet name="ic_login++" r:id="rId21" sheetId="19"/>
+    <sheet name="DB_connection_master++" r:id="rId22" sheetId="20"/>
+    <sheet name="icGiftCardVerificationSender++" r:id="rId23" sheetId="21"/>
+    <sheet name="ic_CashDepositPayment++" r:id="rId24" sheetId="22"/>
+    <sheet name="CreateaccountBackend++" r:id="rId25" sheetId="23"/>
+    <sheet name="accountCreation++" r:id="rId26" sheetId="24"/>
+    <sheet name="Russels" r:id="rId27" sheetId="25"/>
+    <sheet name="Login++" r:id="rId28" sheetId="26"/>
+    <sheet name="Bradlows" r:id="rId29" sheetId="27"/>
+    <sheet name="Rochester" r:id="rId30" sheetId="28"/>
+    <sheet name="Sleepmasters" r:id="rId31" sheetId="29"/>
+    <sheet name="HiFiCorp" r:id="rId32" sheetId="30"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2974" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2980" uniqueCount="355">
   <si>
     <t>TCID</t>
   </si>
@@ -495,6 +496,15 @@
     <t>Gift Card Redeem - Registered user</t>
   </si>
   <si>
+    <t>LetterEmail</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>AlanDCoreyrhyta.com</t>
+  </si>
+  <si>
     <t>Paytype_Option</t>
   </si>
   <si>
@@ -639,9 +649,6 @@
     <t>Pending Payment</t>
   </si>
   <si>
-    <t>3100001253</t>
-  </si>
-  <si>
     <t>3100000680</t>
   </si>
   <si>
@@ -873,7 +880,7 @@
     <t>Backend_Lastname</t>
   </si>
   <si>
-    <t>fake608272263561677@automationjdg.co.za</t>
+    <t>fake412663849335371@automationjdg.co.za</t>
   </si>
   <si>
     <t>7503226018089</t>
@@ -882,10 +889,10 @@
     <t>Main Website</t>
   </si>
   <si>
-    <t>fake523543956504195@automationjdg.co.za</t>
-  </si>
-  <si>
-    <t>fake245240200392343@automationjdg.co.za</t>
+    <t>fake868051075740075@automationjdg.co.za</t>
+  </si>
+  <si>
+    <t>fake346708734661735@automationjdg.co.za</t>
   </si>
   <si>
     <t>abcd1234</t>
@@ -936,7 +943,7 @@
     <t>Jones</t>
   </si>
   <si>
-    <t>fake237555351777407@automationjdg.co.za</t>
+    <t>fake234775323367597@automationjdg.co.za</t>
   </si>
   <si>
     <t>2222224</t>
@@ -951,7 +958,7 @@
     <t>5311266534086</t>
   </si>
   <si>
-    <t>fake412521087024036@automationjdg.co.za</t>
+    <t>fake758727078718053@automationjdg.co.za</t>
   </si>
   <si>
     <t>9708027466084</t>
@@ -963,13 +970,13 @@
     <t>5311ABGF25</t>
   </si>
   <si>
-    <t>fake426406610818229@automationjdg.co.za</t>
+    <t>fake571162171152678@automationjdg.co.za</t>
   </si>
   <si>
     <t>2222226</t>
   </si>
   <si>
-    <t>fake935711881466164@automationjdg.co.za</t>
+    <t>fake706583622016088@automationjdg.co.za</t>
   </si>
   <si>
     <t>2222227</t>
@@ -981,7 +988,7 @@
     <t>Create New Customer - Validate Registration Form - validate Existing Account</t>
   </si>
   <si>
-    <t>fake662216448558420@automationjdg.co.za</t>
+    <t>fake948069503316110@automationjdg.co.za</t>
   </si>
   <si>
     <t>22</t>
@@ -990,7 +997,7 @@
     <t>Create New Customer - Validate Registration Form -Password Field</t>
   </si>
   <si>
-    <t>fake406771358034667@automationjdg.co.za</t>
+    <t>fake351285781311085@automationjdg.co.za</t>
   </si>
   <si>
     <t>23</t>
@@ -999,7 +1006,7 @@
     <t>Create New Customer - Validate Registration Form - SAID Field With Less than 13 Digits</t>
   </si>
   <si>
-    <t>fake605942751898004@automationjdg.co.za</t>
+    <t>fake420211587545662@automationjdg.co.za</t>
   </si>
   <si>
     <t>24</t>
@@ -1008,7 +1015,7 @@
     <t>Create New Customer - Validate Registration Form -- SAID Field With More than 13 Digits</t>
   </si>
   <si>
-    <t>fake551015719973479@automationjdg.co.za</t>
+    <t>fake836170228519407@automationjdg.co.za</t>
   </si>
   <si>
     <t>25</t>
@@ -1017,7 +1024,7 @@
     <t>Create New Customer - Validate Registration Form - Incorrect SAID</t>
   </si>
   <si>
-    <t>fake562222176655286@automationjdg.co.za</t>
+    <t>fake684348512237537@automationjdg.co.za</t>
   </si>
   <si>
     <t>TestCaseID</t>
@@ -1316,6 +1323,229 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I1" t="s">
+        <v>186</v>
+      </c>
+      <c r="J1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G2" t="s">
+        <v>191</v>
+      </c>
+      <c r="H2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I2" t="s">
+        <v>192</v>
+      </c>
+      <c r="J2" t="s">
+        <v>180</v>
+      </c>
+      <c r="K2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F3" t="s">
+        <v>190</v>
+      </c>
+      <c r="G3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I3" t="s">
+        <v>192</v>
+      </c>
+      <c r="J3" t="s">
+        <v>180</v>
+      </c>
+      <c r="K3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F4" t="s">
+        <v>190</v>
+      </c>
+      <c r="G4" t="s">
+        <v>191</v>
+      </c>
+      <c r="H4" t="s">
+        <v>180</v>
+      </c>
+      <c r="I4" t="s">
+        <v>192</v>
+      </c>
+      <c r="J4" t="s">
+        <v>180</v>
+      </c>
+      <c r="K4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F5" t="s">
+        <v>190</v>
+      </c>
+      <c r="G5" t="s">
+        <v>191</v>
+      </c>
+      <c r="H5" t="s">
+        <v>180</v>
+      </c>
+      <c r="I5" t="s">
+        <v>192</v>
+      </c>
+      <c r="J5" t="s">
+        <v>180</v>
+      </c>
+      <c r="K5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>189</v>
+      </c>
+      <c r="F6" t="s">
+        <v>190</v>
+      </c>
+      <c r="G6" t="s">
+        <v>191</v>
+      </c>
+      <c r="H6" t="s">
+        <v>180</v>
+      </c>
+      <c r="I6" t="s">
+        <v>192</v>
+      </c>
+      <c r="J6" t="s">
+        <v>180</v>
+      </c>
+      <c r="K6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1394,10 +1624,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -1579,7 +1809,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -1598,13 +1828,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="F1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2">
@@ -1621,7 +1851,7 @@
         <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -1641,7 +1871,7 @@
         <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -1661,7 +1891,7 @@
         <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -1681,7 +1911,7 @@
         <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -1689,10 +1919,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -1701,7 +1931,7 @@
         <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -1721,7 +1951,7 @@
         <v>52</v>
       </c>
       <c r="E7" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
@@ -1741,7 +1971,7 @@
         <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
@@ -1761,7 +1991,7 @@
         <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
@@ -1781,7 +2011,7 @@
         <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
@@ -1832,7 +2062,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E16"/>
   <sheetViews>
@@ -1851,10 +2081,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2">
@@ -1871,7 +2101,7 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3">
@@ -1888,7 +2118,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4">
@@ -1905,7 +2135,7 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5">
@@ -1922,15 +2152,15 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -1939,7 +2169,7 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7">
@@ -1953,10 +2183,10 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8">
@@ -1973,7 +2203,7 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9">
@@ -1990,7 +2220,7 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10">
@@ -2004,10 +2234,10 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E10" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11">
@@ -2021,10 +2251,10 @@
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E11" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12">
@@ -2038,10 +2268,10 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E12" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13">
@@ -2055,10 +2285,10 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E13" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14">
@@ -2075,7 +2305,7 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15">
@@ -2117,7 +2347,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E32"/>
   <sheetViews>
@@ -2136,10 +2366,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2">
@@ -2153,10 +2383,10 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3">
@@ -2170,10 +2400,10 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E3" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4">
@@ -2187,10 +2417,10 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5">
@@ -2204,10 +2434,10 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E5" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6">
@@ -2221,10 +2451,10 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E6" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7">
@@ -2238,10 +2468,10 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E7" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8">
@@ -2255,10 +2485,10 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E8" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9">
@@ -2272,10 +2502,10 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E9" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10">
@@ -2289,10 +2519,10 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11">
@@ -2306,10 +2536,10 @@
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E11" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12">
@@ -2323,10 +2553,10 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E12" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13">
@@ -2340,10 +2570,10 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E13" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14">
@@ -2357,10 +2587,10 @@
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E14" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15">
@@ -2374,10 +2604,10 @@
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E15" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16">
@@ -2391,10 +2621,10 @@
         <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E16" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17">
@@ -2408,10 +2638,10 @@
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E17" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18">
@@ -2425,10 +2655,10 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E18" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19">
@@ -2442,10 +2672,10 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E19" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20">
@@ -2459,10 +2689,10 @@
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E20" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21">
@@ -2476,10 +2706,10 @@
         <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E21" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22">
@@ -2493,10 +2723,10 @@
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E22" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23">
@@ -2510,10 +2740,10 @@
         <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24">
@@ -2527,10 +2757,10 @@
         <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E24" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25">
@@ -2544,27 +2774,27 @@
         <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E25" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B26" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E26" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27">
@@ -2578,10 +2808,10 @@
         <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E27" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28">
@@ -2595,10 +2825,10 @@
         <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E28" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29">
@@ -2612,10 +2842,10 @@
         <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E29" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30">
@@ -2629,10 +2859,10 @@
         <v>11</v>
       </c>
       <c r="D30" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E30" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31">
@@ -2646,10 +2876,10 @@
         <v>11</v>
       </c>
       <c r="D31" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E31" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32">
@@ -2663,10 +2893,10 @@
         <v>11</v>
       </c>
       <c r="D32" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E32" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2674,7 +2904,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -2693,7 +2923,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2">
@@ -2754,10 +2984,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -2777,7 +3007,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
@@ -2911,7 +3141,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -2930,16 +3160,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="F1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="G1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2">
@@ -2953,10 +3183,10 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F2" t="s">
         <v>92</v>
@@ -2976,10 +3206,10 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E3" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F3" t="s">
         <v>92</v>
@@ -2999,13 +3229,13 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E4" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F4" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G4" t="s">
         <v>83</v>
@@ -3022,10 +3252,10 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E5" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F5" t="s">
         <v>92</v>
@@ -3036,19 +3266,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E6" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F6" t="s">
         <v>92</v>
@@ -3068,10 +3298,10 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E7" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="F7" t="s">
         <v>92</v>
@@ -3091,10 +3321,10 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E8" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F8" t="s">
         <v>92</v>
@@ -3114,10 +3344,10 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E9" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F9" t="s">
         <v>92</v>
@@ -3137,13 +3367,13 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E10" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="F10" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="G10" t="s">
         <v>83</v>
@@ -3160,13 +3390,13 @@
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E11" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F11" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G11" t="s">
         <v>83</v>
@@ -3183,13 +3413,13 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E12" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F12" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="G12" t="s">
         <v>83</v>
@@ -3206,10 +3436,10 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E13" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F13" t="s">
         <v>92</v>
@@ -3229,10 +3459,10 @@
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E14" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F14" t="s">
         <v>92</v>
@@ -3252,10 +3482,10 @@
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E15" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F15" t="s">
         <v>92</v>
@@ -3275,10 +3505,10 @@
         <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E16" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F16" t="s">
         <v>92</v>
@@ -3298,10 +3528,10 @@
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E17" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F17" t="s">
         <v>92</v>
@@ -3321,10 +3551,10 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E18" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F18" t="s">
         <v>92</v>
@@ -3344,10 +3574,10 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E19" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F19" t="s">
         <v>92</v>
@@ -3367,10 +3597,10 @@
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E20" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F20" t="s">
         <v>92</v>
@@ -3390,10 +3620,10 @@
         <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E21" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F21" t="s">
         <v>92</v>
@@ -3413,10 +3643,10 @@
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E22" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F22" t="s">
         <v>92</v>
@@ -3436,10 +3666,10 @@
         <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E23" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F23" t="s">
         <v>92</v>
@@ -3459,10 +3689,10 @@
         <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E24" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F24" t="s">
         <v>92</v>
@@ -3482,10 +3712,10 @@
         <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E25" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F25" t="s">
         <v>92</v>
@@ -3505,10 +3735,10 @@
         <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E26" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F26" t="s">
         <v>92</v>
@@ -3522,7 +3752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -3544,7 +3774,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2">
@@ -3558,10 +3788,10 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3">
@@ -3575,10 +3805,10 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4">
@@ -3592,10 +3822,10 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E4" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5">
@@ -3609,10 +3839,10 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E5" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3620,7 +3850,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -3636,16 +3866,16 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="F1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2">
@@ -3656,16 +3886,16 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3">
@@ -3676,16 +3906,16 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E3" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -3693,7 +3923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E16"/>
   <sheetViews>
@@ -3712,10 +3942,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2">
@@ -3729,10 +3959,10 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3">
@@ -3746,10 +3976,10 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4">
@@ -3763,10 +3993,10 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E4" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5">
@@ -3780,10 +4010,10 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E5" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6">
@@ -3797,10 +4027,10 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E6" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7">
@@ -3814,10 +4044,10 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E7" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8">
@@ -3831,10 +4061,10 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E8" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9">
@@ -3848,10 +4078,10 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E9" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10">
@@ -3970,134 +4200,6 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E1" t="s">
-        <v>202</v>
-      </c>
-      <c r="F1" t="s">
-        <v>203</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" t="s">
-        <v>241</v>
-      </c>
-      <c r="C2" t="s">
-        <v>242</v>
-      </c>
-      <c r="D2" t="s">
-        <v>243</v>
-      </c>
-      <c r="E2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F2" t="s">
-        <v>244</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>245</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>246</v>
-      </c>
-      <c r="B4" t="s">
-        <v>247</v>
-      </c>
-      <c r="C4" t="s">
-        <v>248</v>
-      </c>
-      <c r="D4" t="s">
-        <v>249</v>
-      </c>
-      <c r="E4" t="s">
-        <v>250</v>
-      </c>
-      <c r="F4" t="s">
-        <v>251</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>252</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4723,6 +4825,134 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" t="s">
+        <v>250</v>
+      </c>
+      <c r="D4" t="s">
+        <v>251</v>
+      </c>
+      <c r="E4" t="s">
+        <v>252</v>
+      </c>
+      <c r="F4" t="s">
+        <v>253</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4737,31 +4967,31 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="G1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="H1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="I1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="J1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="K1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2">
@@ -4772,10 +5002,10 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -4787,7 +5017,7 @@
         <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="I2" t="s">
         <v>9</v>
@@ -4807,10 +5037,10 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D3" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -4822,7 +5052,7 @@
         <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="I3" t="s">
         <v>9</v>
@@ -4839,7 +5069,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -4855,10 +5085,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2">
@@ -4869,7 +5099,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -4880,7 +5110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:L13"/>
   <sheetViews>
@@ -4899,31 +5129,31 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="G1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="H1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="I1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="J1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="K1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="L1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2">
@@ -4937,25 +5167,25 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="F2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="G2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="H2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="I2" t="s">
         <v>9</v>
       </c>
       <c r="J2" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="K2" t="s">
         <v>55</v>
@@ -4975,25 +5205,25 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E3" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="F3" t="s">
+        <v>282</v>
+      </c>
+      <c r="G3" t="s">
+        <v>272</v>
+      </c>
+      <c r="H3" t="s">
         <v>280</v>
       </c>
-      <c r="G3" t="s">
-        <v>270</v>
-      </c>
-      <c r="H3" t="s">
-        <v>278</v>
-      </c>
       <c r="I3" t="s">
         <v>9</v>
       </c>
       <c r="J3" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="K3" t="s">
         <v>55</v>
@@ -5013,25 +5243,25 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E4" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="F4" t="s">
+        <v>283</v>
+      </c>
+      <c r="G4" t="s">
+        <v>273</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>284</v>
+      </c>
+      <c r="J4" t="s">
         <v>281</v>
-      </c>
-      <c r="G4" t="s">
-        <v>271</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" t="s">
-        <v>282</v>
-      </c>
-      <c r="J4" t="s">
-        <v>279</v>
       </c>
       <c r="K4" t="s">
         <v>55</v>
@@ -5387,7 +5617,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:S11"/>
   <sheetViews>
@@ -5400,7 +5630,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -5412,46 +5642,46 @@
         <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="G1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="H1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="I1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="J1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="K1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="L1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="M1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="N1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="O1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="P1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="Q1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="R1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="S1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2">
@@ -5465,37 +5695,37 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F2" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="G2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="I2" t="s">
         <v>49</v>
       </c>
       <c r="J2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="K2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="L2" t="s">
         <v>50</v>
       </c>
       <c r="M2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="N2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="O2" t="s">
         <v>49</v>
@@ -5524,37 +5754,37 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F3" t="s">
+        <v>305</v>
+      </c>
+      <c r="G3" t="s">
+        <v>239</v>
+      </c>
+      <c r="H3" t="s">
+        <v>239</v>
+      </c>
+      <c r="I3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" t="s">
+        <v>301</v>
+      </c>
+      <c r="K3" t="s">
+        <v>302</v>
+      </c>
+      <c r="L3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" t="s">
         <v>303</v>
       </c>
-      <c r="G3" t="s">
-        <v>237</v>
-      </c>
-      <c r="H3" t="s">
-        <v>237</v>
-      </c>
-      <c r="I3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J3" t="s">
-        <v>299</v>
-      </c>
-      <c r="K3" t="s">
-        <v>300</v>
-      </c>
-      <c r="L3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M3" t="s">
-        <v>301</v>
-      </c>
       <c r="N3" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="O3" t="s">
         <v>50</v>
@@ -5583,37 +5813,37 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E4" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F4" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="G4" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H4" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="I4" t="s">
         <v>50</v>
       </c>
       <c r="J4" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="K4" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="L4" t="s">
         <v>50</v>
       </c>
       <c r="M4" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="N4" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="O4" t="s">
         <v>50</v>
@@ -5642,37 +5872,37 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E5" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F5" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="G5" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H5" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="I5" t="s">
         <v>50</v>
       </c>
       <c r="J5" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="K5" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="L5" t="s">
         <v>49</v>
       </c>
       <c r="M5" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="N5" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="O5" t="s">
         <v>50</v>
@@ -5701,37 +5931,37 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E6" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F6" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="G6" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H6" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="I6" t="s">
         <v>50</v>
       </c>
       <c r="J6" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="K6" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="L6" t="s">
         <v>50</v>
       </c>
       <c r="M6" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="N6" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="O6" t="s">
         <v>50</v>
@@ -5751,46 +5981,46 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>298</v>
+      </c>
+      <c r="E7" t="s">
+        <v>299</v>
+      </c>
+      <c r="F7" t="s">
+        <v>315</v>
+      </c>
+      <c r="G7" t="s">
+        <v>239</v>
+      </c>
+      <c r="H7" t="s">
+        <v>239</v>
+      </c>
+      <c r="I7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" t="s">
         <v>312</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>296</v>
-      </c>
-      <c r="E7" t="s">
-        <v>297</v>
-      </c>
-      <c r="F7" t="s">
-        <v>313</v>
-      </c>
-      <c r="G7" t="s">
-        <v>237</v>
-      </c>
-      <c r="H7" t="s">
-        <v>237</v>
-      </c>
-      <c r="I7" t="s">
-        <v>50</v>
-      </c>
-      <c r="J7" t="s">
-        <v>310</v>
-      </c>
       <c r="K7" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="L7" t="s">
         <v>50</v>
       </c>
       <c r="M7" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="N7" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="O7" t="s">
         <v>49</v>
@@ -5810,46 +6040,46 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B8" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E8" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F8" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="G8" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H8" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="I8" t="s">
         <v>50</v>
       </c>
       <c r="J8" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="K8" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="L8" t="s">
         <v>50</v>
       </c>
       <c r="M8" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="N8" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="O8" t="s">
         <v>50</v>
@@ -5869,46 +6099,46 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B9" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E9" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F9" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="G9" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H9" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="I9" t="s">
         <v>50</v>
       </c>
       <c r="J9" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="K9" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="L9" t="s">
         <v>50</v>
       </c>
       <c r="M9" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="N9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="O9" t="s">
         <v>50</v>
@@ -5928,46 +6158,46 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B10" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E10" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F10" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="G10" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H10" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="I10" t="s">
         <v>50</v>
       </c>
       <c r="J10" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="K10" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="L10" t="s">
         <v>50</v>
       </c>
       <c r="M10" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="N10" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="O10" t="s">
         <v>50</v>
@@ -5987,46 +6217,46 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B11" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E11" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F11" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="G11" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H11" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="I11" t="s">
         <v>50</v>
       </c>
       <c r="J11" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="K11" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="L11" t="s">
         <v>50</v>
       </c>
       <c r="M11" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="N11" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="O11" t="s">
         <v>50</v>
@@ -6049,7 +6279,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -6059,69 +6289,69 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D1" t="s">
         <v>109</v>
       </c>
       <c r="E1" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="F1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="G1" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="H1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="I1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="J1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="K1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="L1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="M1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="N1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D2" t="s">
         <v>85</v>
       </c>
       <c r="E2" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="F2" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="G2" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
@@ -6147,22 +6377,22 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="F3" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -6194,7 +6424,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -6210,10 +6440,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2">
@@ -6224,10 +6454,10 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D2" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3">
@@ -6238,10 +6468,10 @@
         <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D3" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4">
@@ -6252,10 +6482,10 @@
         <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D4" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5">
@@ -6266,10 +6496,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D5" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="6">
@@ -6280,10 +6510,10 @@
         <v>92</v>
       </c>
       <c r="C6" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D6" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7">
@@ -6294,10 +6524,10 @@
         <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D7" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8">
@@ -6308,10 +6538,10 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D8" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9">
@@ -6322,10 +6552,10 @@
         <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D9" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10">
@@ -6336,10 +6566,10 @@
         <v>81</v>
       </c>
       <c r="C10" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D10" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11">
@@ -6350,10 +6580,10 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D11" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="12">
@@ -6364,10 +6594,10 @@
         <v>92</v>
       </c>
       <c r="C12" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D12" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13">
@@ -6378,146 +6608,10 @@
         <v>81</v>
       </c>
       <c r="C13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D13" t="s">
-        <v>346</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>326</v>
-      </c>
-      <c r="B1" t="s">
-        <v>328</v>
-      </c>
-      <c r="C1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" t="s">
-        <v>329</v>
-      </c>
-      <c r="E1" t="s">
-        <v>330</v>
-      </c>
-      <c r="F1" t="s">
-        <v>331</v>
-      </c>
-      <c r="G1" t="s">
-        <v>332</v>
-      </c>
-      <c r="H1" t="s">
-        <v>333</v>
-      </c>
-      <c r="I1" t="s">
-        <v>334</v>
-      </c>
-      <c r="J1" t="s">
-        <v>335</v>
-      </c>
-      <c r="K1" t="s">
-        <v>336</v>
-      </c>
-      <c r="L1" t="s">
-        <v>337</v>
-      </c>
-      <c r="M1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>349</v>
-      </c>
-      <c r="C2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" t="s">
-        <v>350</v>
-      </c>
-      <c r="E2" t="s">
-        <v>351</v>
-      </c>
-      <c r="F2" t="s">
-        <v>352</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" t="s">
-        <v>349</v>
-      </c>
-      <c r="C3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D3" t="s">
-        <v>350</v>
-      </c>
-      <c r="E3" t="s">
-        <v>351</v>
-      </c>
-      <c r="F3" t="s">
-        <v>352</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" t="s">
-        <v>9</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -6535,43 +6629,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C1" t="s">
         <v>109</v>
       </c>
       <c r="D1" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="F1" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="G1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="H1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="J1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="K1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="L1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="M1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2">
@@ -6579,19 +6673,19 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C2" t="s">
         <v>85</v>
       </c>
       <c r="D2" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E2" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F2" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -6620,19 +6714,19 @@
         <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C3" t="s">
         <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E3" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F3" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -6671,43 +6765,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C1" t="s">
         <v>109</v>
       </c>
       <c r="D1" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="F1" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="G1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="H1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="J1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="K1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="L1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="M1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2">
@@ -6715,19 +6809,19 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C2" t="s">
         <v>85</v>
       </c>
       <c r="D2" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E2" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F2" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -6756,19 +6850,19 @@
         <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C3" t="s">
         <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E3" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F3" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -6807,43 +6901,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C1" t="s">
         <v>109</v>
       </c>
       <c r="D1" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="F1" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="G1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="H1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="J1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="K1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="L1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="M1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2">
@@ -6851,19 +6945,19 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C2" t="s">
         <v>85</v>
       </c>
       <c r="D2" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E2" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F2" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -6892,19 +6986,19 @@
         <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C3" t="s">
         <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E3" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F3" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -9171,6 +9265,142 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F1" t="s">
+        <v>333</v>
+      </c>
+      <c r="G1" t="s">
+        <v>334</v>
+      </c>
+      <c r="H1" t="s">
+        <v>335</v>
+      </c>
+      <c r="I1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K1" t="s">
+        <v>338</v>
+      </c>
+      <c r="L1" t="s">
+        <v>339</v>
+      </c>
+      <c r="M1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" t="s">
+        <v>352</v>
+      </c>
+      <c r="E2" t="s">
+        <v>353</v>
+      </c>
+      <c r="F2" t="s">
+        <v>354</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s">
+        <v>352</v>
+      </c>
+      <c r="E3" t="s">
+        <v>353</v>
+      </c>
+      <c r="F3" t="s">
+        <v>354</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E22"/>
@@ -10259,6 +10489,41 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10276,7 +10541,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2">
@@ -10290,7 +10555,7 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3">
@@ -10304,7 +10569,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4">
@@ -10318,7 +10583,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5">
@@ -10332,21 +10597,21 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7">
@@ -10360,7 +10625,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8">
@@ -10374,7 +10639,7 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9">
@@ -10388,7 +10653,7 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10">
@@ -10402,7 +10667,7 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11">
@@ -10416,7 +10681,7 @@
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12">
@@ -10430,7 +10695,7 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -10438,7 +10703,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:N9"/>
   <sheetViews>
@@ -10457,37 +10722,37 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E1" t="s">
         <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="H1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="I1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="J1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="K1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="L1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="M1" t="s">
         <v>28</v>
       </c>
       <c r="N1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2">
@@ -10501,37 +10766,37 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H2" t="s">
         <v>72</v>
       </c>
       <c r="I2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="J2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="K2" t="s">
+        <v>174</v>
+      </c>
+      <c r="L2" t="s">
         <v>171</v>
       </c>
-      <c r="L2" t="s">
-        <v>168</v>
-      </c>
       <c r="M2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="N2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3">
@@ -10545,37 +10810,37 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H3" t="s">
         <v>72</v>
       </c>
       <c r="I3" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="J3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="K3" t="s">
+        <v>174</v>
+      </c>
+      <c r="L3" t="s">
         <v>171</v>
       </c>
-      <c r="L3" t="s">
-        <v>168</v>
-      </c>
       <c r="M3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="N3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4">
@@ -10589,37 +10854,37 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E4" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G4" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H4" t="s">
         <v>72</v>
       </c>
       <c r="I4" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="J4" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="K4" t="s">
+        <v>174</v>
+      </c>
+      <c r="L4" t="s">
         <v>171</v>
       </c>
-      <c r="L4" t="s">
-        <v>168</v>
-      </c>
       <c r="M4" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="N4" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5">
@@ -10633,81 +10898,81 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E5" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F5" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G5" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H5" t="s">
         <v>72</v>
       </c>
       <c r="I5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="J5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="K5" t="s">
+        <v>174</v>
+      </c>
+      <c r="L5" t="s">
         <v>171</v>
       </c>
-      <c r="L5" t="s">
-        <v>168</v>
-      </c>
       <c r="M5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="N5" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F6" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G6" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H6" t="s">
         <v>72</v>
       </c>
       <c r="I6" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="J6" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="K6" t="s">
+        <v>174</v>
+      </c>
+      <c r="L6" t="s">
         <v>171</v>
       </c>
-      <c r="L6" t="s">
-        <v>168</v>
-      </c>
       <c r="M6" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="N6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7">
@@ -10721,37 +10986,37 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E7" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F7" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H7" t="s">
         <v>72</v>
       </c>
       <c r="I7" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="J7" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="K7" t="s">
+        <v>174</v>
+      </c>
+      <c r="L7" t="s">
         <v>171</v>
       </c>
-      <c r="L7" t="s">
-        <v>168</v>
-      </c>
       <c r="M7" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="N7" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8">
@@ -10765,37 +11030,37 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E8" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F8" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G8" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H8" t="s">
         <v>72</v>
       </c>
       <c r="I8" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="J8" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="K8" t="s">
+        <v>174</v>
+      </c>
+      <c r="L8" t="s">
         <v>171</v>
       </c>
-      <c r="L8" t="s">
-        <v>168</v>
-      </c>
       <c r="M8" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="N8" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9">
@@ -10809,260 +11074,37 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E9" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F9" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H9" t="s">
         <v>72</v>
       </c>
       <c r="I9" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="J9" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="K9" t="s">
+        <v>174</v>
+      </c>
+      <c r="L9" t="s">
         <v>171</v>
       </c>
-      <c r="L9" t="s">
-        <v>168</v>
-      </c>
       <c r="M9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="N9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E1" t="s">
         <v>179</v>
-      </c>
-      <c r="F1" t="s">
-        <v>180</v>
-      </c>
-      <c r="G1" t="s">
-        <v>181</v>
-      </c>
-      <c r="H1" t="s">
-        <v>182</v>
-      </c>
-      <c r="I1" t="s">
-        <v>183</v>
-      </c>
-      <c r="J1" t="s">
-        <v>184</v>
-      </c>
-      <c r="K1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H2" t="s">
-        <v>177</v>
-      </c>
-      <c r="I2" t="s">
-        <v>189</v>
-      </c>
-      <c r="J2" t="s">
-        <v>177</v>
-      </c>
-      <c r="K2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" t="s">
-        <v>186</v>
-      </c>
-      <c r="F3" t="s">
-        <v>187</v>
-      </c>
-      <c r="G3" t="s">
-        <v>188</v>
-      </c>
-      <c r="H3" t="s">
-        <v>177</v>
-      </c>
-      <c r="I3" t="s">
-        <v>189</v>
-      </c>
-      <c r="J3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" t="s">
-        <v>186</v>
-      </c>
-      <c r="F4" t="s">
-        <v>187</v>
-      </c>
-      <c r="G4" t="s">
-        <v>188</v>
-      </c>
-      <c r="H4" t="s">
-        <v>177</v>
-      </c>
-      <c r="I4" t="s">
-        <v>189</v>
-      </c>
-      <c r="J4" t="s">
-        <v>177</v>
-      </c>
-      <c r="K4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" t="s">
-        <v>186</v>
-      </c>
-      <c r="F5" t="s">
-        <v>187</v>
-      </c>
-      <c r="G5" t="s">
-        <v>188</v>
-      </c>
-      <c r="H5" t="s">
-        <v>177</v>
-      </c>
-      <c r="I5" t="s">
-        <v>189</v>
-      </c>
-      <c r="J5" t="s">
-        <v>177</v>
-      </c>
-      <c r="K5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B6" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" t="s">
-        <v>186</v>
-      </c>
-      <c r="F6" t="s">
-        <v>187</v>
-      </c>
-      <c r="G6" t="s">
-        <v>188</v>
-      </c>
-      <c r="H6" t="s">
-        <v>177</v>
-      </c>
-      <c r="I6" t="s">
-        <v>189</v>
-      </c>
-      <c r="J6" t="s">
-        <v>177</v>
-      </c>
-      <c r="K6" t="s">
-        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TA239 and TA274 (Completed)
TCID 28 In excel sheet = TA274
TCID 30 In excel sheet = TA239(TA275)
</commit_message>
<xml_diff>
--- a/Reports/Datasheet.xlsx
+++ b/Reports/Datasheet.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3604" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3617" uniqueCount="493">
   <si>
     <t>TCID</t>
   </si>
@@ -1130,6 +1130,12 @@
   </si>
   <si>
     <t>1#1#1</t>
+  </si>
+  <si>
+    <t>Add products to cart and clear cart</t>
+  </si>
+  <si>
+    <t>1#1#2</t>
   </si>
   <si>
     <t>scratchCode</t>
@@ -8965,7 +8971,7 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10089,6 +10095,38 @@
       </c>
       <c r="J35" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>360</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>358</v>
+      </c>
+      <c r="F36" t="s">
+        <v>333</v>
+      </c>
+      <c r="G36" t="s">
+        <v>334</v>
+      </c>
+      <c r="H36" t="s">
+        <v>352</v>
+      </c>
+      <c r="I36" t="s">
+        <v>361</v>
+      </c>
+      <c r="J36" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -10118,7 +10156,7 @@
         <v>125</v>
       </c>
       <c r="E1" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="2">
@@ -10132,10 +10170,10 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E2" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3">
@@ -10149,10 +10187,10 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E3" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="4">
@@ -10166,10 +10204,10 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E4" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="5">
@@ -10183,10 +10221,10 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E5" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -10210,16 +10248,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="E1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="F1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2">
@@ -10230,16 +10268,16 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D2" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E2" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="F2" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3">
@@ -10250,16 +10288,16 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D3" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E3" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="F3" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -10303,10 +10341,10 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E2" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3">
@@ -10323,7 +10361,7 @@
         <v>288</v>
       </c>
       <c r="E3" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4">
@@ -10340,7 +10378,7 @@
         <v>288</v>
       </c>
       <c r="E4" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="5">
@@ -10357,7 +10395,7 @@
         <v>288</v>
       </c>
       <c r="E5" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="6">
@@ -10371,10 +10409,10 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E6" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7">
@@ -10388,10 +10426,10 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E7" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="8">
@@ -10405,10 +10443,10 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E8" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="9">
@@ -10422,10 +10460,10 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E9" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10">
@@ -10433,7 +10471,7 @@
         <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -10442,7 +10480,7 @@
         <v>88</v>
       </c>
       <c r="E10" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="11">
@@ -10450,7 +10488,7 @@
         <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -10459,7 +10497,7 @@
         <v>88</v>
       </c>
       <c r="E11" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="12">
@@ -10476,7 +10514,7 @@
         <v>88</v>
       </c>
       <c r="E12" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13">
@@ -10493,7 +10531,7 @@
         <v>88</v>
       </c>
       <c r="E13" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="14">
@@ -10510,7 +10548,7 @@
         <v>88</v>
       </c>
       <c r="E14" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15">
@@ -10524,10 +10562,10 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="E15" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="16">
@@ -10565,13 +10603,13 @@
         <v>200</v>
       </c>
       <c r="B1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C1" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D1" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="E1" t="s">
         <v>316</v>
@@ -10588,19 +10626,19 @@
         <v>203</v>
       </c>
       <c r="B2" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="C2" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="D2" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="E2" t="s">
         <v>318</v>
       </c>
       <c r="F2" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="G2" t="s">
         <v>47</v>
@@ -10608,7 +10646,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B3" t="s">
         <v>47</v>
@@ -10631,22 +10669,22 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B4" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C4" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D4" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E4" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="F4" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="G4" t="s">
         <v>47</v>
@@ -10654,7 +10692,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B5" t="s">
         <v>47</v>
@@ -10682,7 +10720,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10729,6 +10767,17 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -10753,31 +10802,31 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="E1" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="F1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="G1" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="H1" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="I1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="J1" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="K1" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="2">
@@ -10791,7 +10840,7 @@
         <v>288</v>
       </c>
       <c r="D2" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="E2" t="s">
         <v>47</v>
@@ -10803,7 +10852,7 @@
         <v>47</v>
       </c>
       <c r="H2" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="I2" t="s">
         <v>47</v>
@@ -10826,7 +10875,7 @@
         <v>288</v>
       </c>
       <c r="D3" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="E3" t="s">
         <v>47</v>
@@ -10838,7 +10887,7 @@
         <v>47</v>
       </c>
       <c r="H3" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="I3" t="s">
         <v>47</v>
@@ -10871,10 +10920,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D1" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2">
@@ -10885,7 +10934,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D2" t="s">
         <v>47</v>
@@ -10915,31 +10964,31 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="E1" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="F1" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="G1" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="H1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="I1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="J1" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="K1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="L1" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="2">
@@ -10953,25 +11002,25 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="E2" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="F2" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="G2" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="H2" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="I2" t="s">
         <v>47</v>
       </c>
       <c r="J2" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="K2" t="s">
         <v>18</v>
@@ -10991,25 +11040,25 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="E3" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="F3" t="s">
+        <v>422</v>
+      </c>
+      <c r="G3" t="s">
+        <v>412</v>
+      </c>
+      <c r="H3" t="s">
         <v>420</v>
       </c>
-      <c r="G3" t="s">
-        <v>410</v>
-      </c>
-      <c r="H3" t="s">
-        <v>418</v>
-      </c>
       <c r="I3" t="s">
         <v>47</v>
       </c>
       <c r="J3" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="K3" t="s">
         <v>18</v>
@@ -11029,25 +11078,25 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="E4" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="F4" t="s">
+        <v>423</v>
+      </c>
+      <c r="G4" t="s">
+        <v>413</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" t="s">
+        <v>424</v>
+      </c>
+      <c r="J4" t="s">
         <v>421</v>
-      </c>
-      <c r="G4" t="s">
-        <v>411</v>
-      </c>
-      <c r="H4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" t="s">
-        <v>422</v>
-      </c>
-      <c r="J4" t="s">
-        <v>419</v>
       </c>
       <c r="K4" t="s">
         <v>18</v>
@@ -11416,7 +11465,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -11428,46 +11477,46 @@
         <v>144</v>
       </c>
       <c r="F1" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="G1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="H1" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="I1" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="J1" t="s">
         <v>275</v>
       </c>
       <c r="K1" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="L1" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="M1" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="N1" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="O1" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="P1" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="Q1" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="R1" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="S1" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2">
@@ -11481,37 +11530,37 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E2" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="F2" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="G2" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="H2" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="I2" t="s">
         <v>43</v>
       </c>
       <c r="J2" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="K2" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="L2" t="s">
         <v>56</v>
       </c>
       <c r="M2" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="N2" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="O2" t="s">
         <v>43</v>
@@ -11540,37 +11589,37 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E3" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="F3" t="s">
+        <v>445</v>
+      </c>
+      <c r="G3" t="s">
+        <v>375</v>
+      </c>
+      <c r="H3" t="s">
+        <v>375</v>
+      </c>
+      <c r="I3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" t="s">
+        <v>441</v>
+      </c>
+      <c r="K3" t="s">
+        <v>442</v>
+      </c>
+      <c r="L3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M3" t="s">
         <v>443</v>
       </c>
-      <c r="G3" t="s">
-        <v>373</v>
-      </c>
-      <c r="H3" t="s">
-        <v>373</v>
-      </c>
-      <c r="I3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" t="s">
-        <v>439</v>
-      </c>
-      <c r="K3" t="s">
-        <v>440</v>
-      </c>
-      <c r="L3" t="s">
-        <v>56</v>
-      </c>
-      <c r="M3" t="s">
-        <v>441</v>
-      </c>
       <c r="N3" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="O3" t="s">
         <v>56</v>
@@ -11599,37 +11648,37 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E4" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="F4" t="s">
         <v>288</v>
       </c>
       <c r="G4" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="H4" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="I4" t="s">
         <v>56</v>
       </c>
       <c r="J4" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="K4" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="L4" t="s">
         <v>56</v>
       </c>
       <c r="M4" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="N4" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="O4" t="s">
         <v>56</v>
@@ -11658,37 +11707,37 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E5" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="F5" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="G5" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="H5" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="I5" t="s">
         <v>56</v>
       </c>
       <c r="J5" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="K5" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="L5" t="s">
         <v>43</v>
       </c>
       <c r="M5" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="N5" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="O5" t="s">
         <v>56</v>
@@ -11717,37 +11766,37 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E6" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="F6" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="G6" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="H6" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="I6" t="s">
         <v>56</v>
       </c>
       <c r="J6" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="K6" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="L6" t="s">
         <v>56</v>
       </c>
       <c r="M6" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="N6" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="O6" t="s">
         <v>56</v>
@@ -11767,46 +11816,46 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="B7" t="s">
+        <v>454</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>438</v>
+      </c>
+      <c r="E7" t="s">
+        <v>439</v>
+      </c>
+      <c r="F7" t="s">
+        <v>455</v>
+      </c>
+      <c r="G7" t="s">
+        <v>375</v>
+      </c>
+      <c r="H7" t="s">
+        <v>375</v>
+      </c>
+      <c r="I7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" t="s">
         <v>452</v>
       </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>436</v>
-      </c>
-      <c r="E7" t="s">
-        <v>437</v>
-      </c>
-      <c r="F7" t="s">
-        <v>453</v>
-      </c>
-      <c r="G7" t="s">
-        <v>373</v>
-      </c>
-      <c r="H7" t="s">
-        <v>373</v>
-      </c>
-      <c r="I7" t="s">
-        <v>56</v>
-      </c>
-      <c r="J7" t="s">
-        <v>450</v>
-      </c>
       <c r="K7" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="L7" t="s">
         <v>56</v>
       </c>
       <c r="M7" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="N7" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="O7" t="s">
         <v>43</v>
@@ -11829,43 +11878,43 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E8" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="F8" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="G8" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="H8" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="I8" t="s">
         <v>56</v>
       </c>
       <c r="J8" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="K8" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="L8" t="s">
         <v>56</v>
       </c>
       <c r="M8" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="N8" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="O8" t="s">
         <v>56</v>
@@ -11885,46 +11934,46 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B9" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E9" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="F9" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="G9" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="H9" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="I9" t="s">
         <v>56</v>
       </c>
       <c r="J9" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="K9" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="L9" t="s">
         <v>56</v>
       </c>
       <c r="M9" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="N9" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="O9" t="s">
         <v>56</v>
@@ -11947,43 +11996,43 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E10" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="F10" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="G10" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="H10" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="I10" t="s">
         <v>56</v>
       </c>
       <c r="J10" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="K10" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="L10" t="s">
         <v>56</v>
       </c>
       <c r="M10" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="N10" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="O10" t="s">
         <v>56</v>
@@ -12003,46 +12052,46 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="B11" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E11" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="F11" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="G11" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="H11" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="I11" t="s">
         <v>56</v>
       </c>
       <c r="J11" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="K11" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="L11" t="s">
         <v>56</v>
       </c>
       <c r="M11" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="N11" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="O11" t="s">
         <v>56</v>
@@ -12075,69 +12124,69 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B1" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="D1" t="s">
         <v>227</v>
       </c>
       <c r="E1" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="F1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="G1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="H1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="I1" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="J1" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="K1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="L1" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="M1" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="N1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B2" t="s">
         <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="D2" t="s">
         <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="F2" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="G2" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="H2" t="s">
         <v>47</v>
@@ -12163,22 +12212,22 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B3" t="s">
         <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="D3" t="s">
         <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="F3" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="G3" t="s">
         <v>47</v>
@@ -12226,10 +12275,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="D1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2">
@@ -12240,10 +12289,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D2" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3">
@@ -12254,10 +12303,10 @@
         <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D3" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="4">
@@ -12268,10 +12317,10 @@
         <v>113</v>
       </c>
       <c r="C4" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D4" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="5">
@@ -12282,10 +12331,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D5" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="6">
@@ -12296,10 +12345,10 @@
         <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D6" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="7">
@@ -12310,10 +12359,10 @@
         <v>113</v>
       </c>
       <c r="C7" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D7" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="8">
@@ -12324,10 +12373,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D8" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="9">
@@ -12338,10 +12387,10 @@
         <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D9" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="10">
@@ -12352,10 +12401,10 @@
         <v>113</v>
       </c>
       <c r="C10" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D10" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="11">
@@ -12366,10 +12415,10 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D11" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="12">
@@ -12380,10 +12429,10 @@
         <v>64</v>
       </c>
       <c r="C12" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D12" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="13">
@@ -12394,10 +12443,10 @@
         <v>113</v>
       </c>
       <c r="C13" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D13" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -12415,43 +12464,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C1" t="s">
         <v>227</v>
       </c>
       <c r="D1" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="E1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="F1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="G1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="H1" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="I1" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="J1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="K1" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="L1" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="M1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="2">
@@ -12459,19 +12508,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C2" t="s">
         <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="E2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="F2" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="G2" t="s">
         <v>47</v>
@@ -12500,19 +12549,19 @@
         <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C3" t="s">
         <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="E3" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="F3" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="G3" t="s">
         <v>47</v>
@@ -12551,43 +12600,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C1" t="s">
         <v>227</v>
       </c>
       <c r="D1" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="E1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="F1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="G1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="H1" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="I1" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="J1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="K1" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="L1" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="M1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="2">
@@ -12595,19 +12644,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C2" t="s">
         <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="E2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="F2" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="G2" t="s">
         <v>47</v>
@@ -12636,19 +12685,19 @@
         <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C3" t="s">
         <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="E3" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="F3" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="G3" t="s">
         <v>47</v>
@@ -12687,43 +12736,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C1" t="s">
         <v>227</v>
       </c>
       <c r="D1" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="E1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="F1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="G1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="H1" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="I1" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="J1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="K1" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="L1" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="M1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="2">
@@ -12731,19 +12780,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C2" t="s">
         <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="E2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="F2" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="G2" t="s">
         <v>47</v>
@@ -12772,19 +12821,19 @@
         <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C3" t="s">
         <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="E3" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="F3" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="G3" t="s">
         <v>47</v>
@@ -12823,43 +12872,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C1" t="s">
         <v>227</v>
       </c>
       <c r="D1" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="E1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="F1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="G1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="H1" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="I1" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="J1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="K1" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="L1" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="M1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="2">
@@ -12867,19 +12916,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C2" t="s">
         <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="E2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="F2" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="G2" t="s">
         <v>47</v>
@@ -12908,19 +12957,19 @@
         <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C3" t="s">
         <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="E3" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="F3" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="G3" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Unfinished branch moving to remote jenkins environment
</commit_message>
<xml_diff>
--- a/Reports/Datasheet.xlsx
+++ b/Reports/Datasheet.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3501" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3512" uniqueCount="474">
   <si>
     <t>TCID</t>
   </si>
@@ -1195,6 +1195,9 @@
   </si>
   <si>
     <t>Xpath@123</t>
+  </si>
+  <si>
+    <t>56</t>
   </si>
   <si>
     <t>Test Case name</t>
@@ -10156,7 +10159,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10299,6 +10302,41 @@
         <v>43</v>
       </c>
       <c r="K4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>382</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5" t="s">
+        <v>381</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>378</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -10531,10 +10569,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2">
@@ -10545,7 +10583,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D2" t="s">
         <v>43</v>
@@ -10575,31 +10613,31 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="F1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="G1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="H1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="I1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="J1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="K1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="L1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2">
@@ -10613,25 +10651,25 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="F2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="G2" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="H2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="I2" t="s">
         <v>43</v>
       </c>
       <c r="J2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="K2" t="s">
         <v>18</v>
@@ -10651,25 +10689,25 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E3" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="F3" t="s">
+        <v>400</v>
+      </c>
+      <c r="G3" t="s">
+        <v>390</v>
+      </c>
+      <c r="H3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" t="s">
         <v>399</v>
-      </c>
-      <c r="G3" t="s">
-        <v>389</v>
-      </c>
-      <c r="H3" t="s">
-        <v>397</v>
-      </c>
-      <c r="I3" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" t="s">
-        <v>398</v>
       </c>
       <c r="K3" t="s">
         <v>18</v>
@@ -10689,25 +10727,25 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="F4" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="G4" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H4" t="s">
         <v>43</v>
       </c>
       <c r="I4" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="J4" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="K4" t="s">
         <v>18</v>
@@ -11076,7 +11114,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -11088,46 +11126,46 @@
         <v>140</v>
       </c>
       <c r="F1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G1" t="s">
         <v>370</v>
       </c>
       <c r="H1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="I1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="J1" t="s">
         <v>272</v>
       </c>
       <c r="K1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="L1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="N1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="O1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="P1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="Q1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="R1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="S1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="2">
@@ -11141,13 +11179,13 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="G2" t="s">
         <v>351</v>
@@ -11159,19 +11197,19 @@
         <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="K2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L2" t="s">
         <v>52</v>
       </c>
       <c r="M2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="O2" t="s">
         <v>39</v>
@@ -11200,13 +11238,13 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="G3" t="s">
         <v>351</v>
@@ -11218,19 +11256,19 @@
         <v>52</v>
       </c>
       <c r="J3" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="K3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L3" t="s">
         <v>52</v>
       </c>
       <c r="M3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="O3" t="s">
         <v>52</v>
@@ -11259,10 +11297,10 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E4" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F4" t="s">
         <v>285</v>
@@ -11277,19 +11315,19 @@
         <v>52</v>
       </c>
       <c r="J4" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="K4" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L4" t="s">
         <v>52</v>
       </c>
       <c r="M4" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="N4" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="O4" t="s">
         <v>52</v>
@@ -11318,13 +11356,13 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E5" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F5" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="G5" t="s">
         <v>351</v>
@@ -11336,19 +11374,19 @@
         <v>52</v>
       </c>
       <c r="J5" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="K5" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L5" t="s">
         <v>39</v>
       </c>
       <c r="M5" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N5" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="O5" t="s">
         <v>52</v>
@@ -11377,13 +11415,13 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E6" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F6" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="G6" t="s">
         <v>351</v>
@@ -11395,19 +11433,19 @@
         <v>52</v>
       </c>
       <c r="J6" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="K6" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L6" t="s">
         <v>52</v>
       </c>
       <c r="M6" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N6" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="O6" t="s">
         <v>52</v>
@@ -11427,22 +11465,22 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B7" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E7" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F7" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="G7" t="s">
         <v>351</v>
@@ -11454,19 +11492,19 @@
         <v>52</v>
       </c>
       <c r="J7" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="K7" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L7" t="s">
         <v>52</v>
       </c>
       <c r="M7" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N7" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="O7" t="s">
         <v>39</v>
@@ -11486,22 +11524,22 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B8" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E8" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F8" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G8" t="s">
         <v>351</v>
@@ -11513,19 +11551,19 @@
         <v>52</v>
       </c>
       <c r="J8" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="K8" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L8" t="s">
         <v>52</v>
       </c>
       <c r="M8" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N8" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="O8" t="s">
         <v>52</v>
@@ -11545,22 +11583,22 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B9" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E9" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F9" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="G9" t="s">
         <v>351</v>
@@ -11572,19 +11610,19 @@
         <v>52</v>
       </c>
       <c r="J9" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="K9" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L9" t="s">
         <v>52</v>
       </c>
       <c r="M9" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N9" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="O9" t="s">
         <v>52</v>
@@ -11604,22 +11642,22 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B10" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E10" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F10" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="G10" t="s">
         <v>351</v>
@@ -11631,19 +11669,19 @@
         <v>52</v>
       </c>
       <c r="J10" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="K10" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L10" t="s">
         <v>52</v>
       </c>
       <c r="M10" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N10" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="O10" t="s">
         <v>52</v>
@@ -11663,22 +11701,22 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B11" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E11" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F11" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="G11" t="s">
         <v>351</v>
@@ -11690,19 +11728,19 @@
         <v>52</v>
       </c>
       <c r="J11" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="K11" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L11" t="s">
         <v>52</v>
       </c>
       <c r="M11" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N11" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="O11" t="s">
         <v>52</v>
@@ -11722,7 +11760,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B12" t="s">
         <v>201</v>
@@ -11731,10 +11769,10 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E12" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F12" t="s">
         <v>285</v>
@@ -11749,19 +11787,19 @@
         <v>52</v>
       </c>
       <c r="J12" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="K12" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L12" t="s">
         <v>52</v>
       </c>
       <c r="M12" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="N12" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="O12" t="s">
         <v>52</v>
@@ -11790,10 +11828,10 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E13" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F13" t="s">
         <v>380</v>
@@ -11808,19 +11846,19 @@
         <v>52</v>
       </c>
       <c r="J13" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="K13" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L13" t="s">
         <v>52</v>
       </c>
       <c r="M13" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="N13" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="O13" t="s">
         <v>52</v>
@@ -11853,69 +11891,69 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D1" t="s">
         <v>223</v>
       </c>
       <c r="E1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="F1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="G1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="H1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="I1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="J1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="L1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="M1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="N1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D2" t="s">
         <v>86</v>
       </c>
       <c r="E2" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="F2" t="s">
+        <v>463</v>
+      </c>
+      <c r="G2" t="s">
         <v>462</v>
-      </c>
-      <c r="G2" t="s">
-        <v>461</v>
       </c>
       <c r="H2" t="s">
         <v>43</v>
@@ -11947,16 +11985,16 @@
         <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D3" t="s">
         <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="F3" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="G3" t="s">
         <v>43</v>
@@ -12004,7 +12042,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D1" t="s">
         <v>370</v>
@@ -12018,10 +12056,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D2" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="3">
@@ -12032,10 +12070,10 @@
         <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D3" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="4">
@@ -12046,10 +12084,10 @@
         <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D4" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="5">
@@ -12060,10 +12098,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D5" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="6">
@@ -12074,10 +12112,10 @@
         <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D6" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="7">
@@ -12088,10 +12126,10 @@
         <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D7" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="8">
@@ -12102,10 +12140,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D8" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="9">
@@ -12116,10 +12154,10 @@
         <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D9" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="10">
@@ -12130,10 +12168,10 @@
         <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D10" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="11">
@@ -12144,10 +12182,10 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D11" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="12">
@@ -12158,10 +12196,10 @@
         <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D12" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="13">
@@ -12172,10 +12210,10 @@
         <v>109</v>
       </c>
       <c r="C13" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D13" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -12193,43 +12231,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C1" t="s">
         <v>223</v>
       </c>
       <c r="D1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="H1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="I1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="J1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="K1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="L1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="M1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="2">
@@ -12237,19 +12275,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C2" t="s">
         <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G2" t="s">
         <v>43</v>
@@ -12278,19 +12316,19 @@
         <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C3" t="s">
         <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E3" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F3" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G3" t="s">
         <v>43</v>
@@ -12329,43 +12367,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C1" t="s">
         <v>223</v>
       </c>
       <c r="D1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="H1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="I1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="J1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="K1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="L1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="M1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="2">
@@ -12373,19 +12411,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C2" t="s">
         <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G2" t="s">
         <v>43</v>
@@ -12414,19 +12452,19 @@
         <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C3" t="s">
         <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E3" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F3" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G3" t="s">
         <v>43</v>
@@ -12465,43 +12503,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C1" t="s">
         <v>223</v>
       </c>
       <c r="D1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="H1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="I1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="J1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="K1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="L1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="M1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="2">
@@ -12509,19 +12547,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C2" t="s">
         <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G2" t="s">
         <v>43</v>
@@ -12550,19 +12588,19 @@
         <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C3" t="s">
         <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E3" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F3" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G3" t="s">
         <v>43</v>
@@ -12601,43 +12639,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C1" t="s">
         <v>223</v>
       </c>
       <c r="D1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="H1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="I1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="J1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="K1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="L1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="M1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="2">
@@ -12645,19 +12683,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C2" t="s">
         <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G2" t="s">
         <v>43</v>
@@ -12686,19 +12724,19 @@
         <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C3" t="s">
         <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E3" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F3" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G3" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Added TA651 Test data to main sheet
</commit_message>
<xml_diff>
--- a/Reports/Datasheet.xlsx
+++ b/Reports/Datasheet.xlsx
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16538" uniqueCount="1420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16614" uniqueCount="1420">
   <si>
     <t>testSuitID</t>
   </si>
@@ -2086,7 +2086,7 @@
     <t>newPassword</t>
   </si>
   <si>
-    <t>S!s9352889446</t>
+    <t>S!s3837972525</t>
   </si>
   <si>
     <t>waitTimeForforgotPasswordEmailInSec</t>
@@ -2191,7 +2191,7 @@
     <t>Beast</t>
   </si>
   <si>
-    <t>fake251036309179362@automationjdg.co.za</t>
+    <t>fake340391342234635@automationjdg.co.za</t>
   </si>
   <si>
     <t>0826996708</t>
@@ -2212,7 +2212,7 @@
     <t>Cash</t>
   </si>
   <si>
-    <t>fake057137112375431@automationjdg.co.za</t>
+    <t>fake695758613158205@automationjdg.co.za</t>
   </si>
   <si>
     <t>0761233216</t>
@@ -2227,7 +2227,7 @@
     <t>Kwem</t>
   </si>
   <si>
-    <t>fake334170319323348@automationjdg.co.za</t>
+    <t>fake336650566151081@automationjdg.co.za</t>
   </si>
   <si>
     <t>0726456547</t>
@@ -2422,10 +2422,10 @@
     <t>Test@gmail.com</t>
   </si>
   <si>
-    <t>fake135564101414752@automationjdg.co.za</t>
-  </si>
-  <si>
-    <t>fake403310393360600@automationjdg.co.za</t>
+    <t>fake485387627879390@automationjdg.co.za</t>
+  </si>
+  <si>
+    <t>fake482156532567521@automationjdg.co.za</t>
   </si>
   <si>
     <t>ProductSelectionType</t>
@@ -3058,7 +3058,7 @@
     <t>Validate_Password_Field</t>
   </si>
   <si>
-    <t>fake306447026087310@automationjdg.co.za</t>
+    <t>fake274329538952502@automationjdg.co.za</t>
   </si>
   <si>
     <t>0823646475</t>
@@ -3076,7 +3076,7 @@
     <t>Jones</t>
   </si>
   <si>
-    <t>fake453430062395034@automationjdg.co.za</t>
+    <t>fake689334065144844@automationjdg.co.za</t>
   </si>
   <si>
     <t>2222227</t>
@@ -3091,10 +3091,10 @@
     <t>5311266534086</t>
   </si>
   <si>
-    <t>fake761097616627616@automationjdg.co.za</t>
-  </si>
-  <si>
-    <t>fake667413900605162@automationjdg.co.za</t>
+    <t>fake318675798086330@automationjdg.co.za</t>
+  </si>
+  <si>
+    <t>fake777723853313327@automationjdg.co.za</t>
   </si>
   <si>
     <t>Cindy</t>
@@ -3103,7 +3103,7 @@
     <t>Smith</t>
   </si>
   <si>
-    <t>fake353115277973812@automationjdg.co.za</t>
+    <t>fake673040420167445@automationjdg.co.za</t>
   </si>
   <si>
     <t>0837849274</t>
@@ -3115,7 +3115,7 @@
     <t>June</t>
   </si>
   <si>
-    <t>fake792401037451912@automationjdg.co.za</t>
+    <t>fake843787028535962@automationjdg.co.za</t>
   </si>
   <si>
     <t>0837849275</t>
@@ -3127,7 +3127,7 @@
     <t>Newslet</t>
   </si>
   <si>
-    <t>fake210778344887807@automationjdg.co.za</t>
+    <t>fake179616234715890@automationjdg.co.za</t>
   </si>
   <si>
     <t>0837849277</t>
@@ -3139,7 +3139,7 @@
     <t>NoNewslet</t>
   </si>
   <si>
-    <t>fake106062314482162@automationjdg.co.za</t>
+    <t>fake726714165470154@automationjdg.co.za</t>
   </si>
   <si>
     <t>0837849278</t>
@@ -3307,7 +3307,7 @@
     <t>Dyson V11 Absolute Extra Vacuum Cleaner</t>
   </si>
   <si>
-    <t>fake633905489553800@automationjdg.co.za</t>
+    <t>fake654879285478167@automationjdg.co.za</t>
   </si>
   <si>
     <t>2222224</t>
@@ -3319,7 +3319,7 @@
     <t>Alice</t>
   </si>
   <si>
-    <t>fake542256146125785@automationjdg.co.za</t>
+    <t>fake693785136243279@automationjdg.co.za</t>
   </si>
   <si>
     <t>0859345893</t>
@@ -3340,7 +3340,7 @@
     <t>Julia</t>
   </si>
   <si>
-    <t>fake502303462010508@automationjdg.co.za</t>
+    <t>fake495923775200185@automationjdg.co.za</t>
   </si>
   <si>
     <t>2222226</t>
@@ -3352,7 +3352,7 @@
     <t>NoNewsLet</t>
   </si>
   <si>
-    <t>fake019584417047590@automationjdg.co.za</t>
+    <t>fake617757144695244@automationjdg.co.za</t>
   </si>
   <si>
     <t>0837849273</t>
@@ -3364,16 +3364,16 @@
     <t>watlevi41@gmail.com</t>
   </si>
   <si>
-    <t>fake450004345105779@automationjdg.co.za</t>
-  </si>
-  <si>
-    <t>fake656285577297173@automationjdg.co.za</t>
-  </si>
-  <si>
-    <t>fake835712128640446@automationjdg.co.za</t>
-  </si>
-  <si>
-    <t>fake056278849048854@automationjdg.co.za</t>
+    <t>fake166694114727896@automationjdg.co.za</t>
+  </si>
+  <si>
+    <t>fake427560262457184@automationjdg.co.za</t>
+  </si>
+  <si>
+    <t>fake246711177582064@automationjdg.co.za</t>
+  </si>
+  <si>
+    <t>fake060794767846180@automationjdg.co.za</t>
   </si>
   <si>
     <t>Validate_Parallel_Login_to_IC</t>
@@ -4108,7 +4108,7 @@
     <t>BackendLast</t>
   </si>
   <si>
-    <t>fake867706477695648@automationjdg.co.za</t>
+    <t>fake534816236772336@automationjdg.co.za</t>
   </si>
   <si>
     <t>9601015800085</t>
@@ -4120,7 +4120,7 @@
     <t>Louw</t>
   </si>
   <si>
-    <t>fake023343789579037@automationjdg.co.za</t>
+    <t>fake657385694639470@automationjdg.co.za</t>
   </si>
   <si>
     <t>9104123240187</t>
@@ -4132,7 +4132,7 @@
     <t>BaLastName</t>
   </si>
   <si>
-    <t>fake288306861831723@automationjdg.co.za</t>
+    <t>fake550612783079512@automationjdg.co.za</t>
   </si>
   <si>
     <t>P1A9SS0P</t>
@@ -21341,7 +21341,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -21543,6 +21543,20 @@
         <v>707</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>614</v>
+      </c>
+      <c r="B15" t="s">
+        <v>615</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>707</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -21550,7 +21564,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -21843,6 +21857,23 @@
       </c>
       <c r="E17" t="s">
         <v>716</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>614</v>
+      </c>
+      <c r="B18" t="s">
+        <v>615</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>715</v>
       </c>
     </row>
   </sheetData>
@@ -21963,7 +21994,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -22906,6 +22937,26 @@
         <v>11</v>
       </c>
       <c r="F47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>614</v>
+      </c>
+      <c r="B48" t="s">
+        <v>615</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>624</v>
+      </c>
+      <c r="E48" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" t="s">
         <v>11</v>
       </c>
     </row>
@@ -26002,7 +26053,7 @@
         <v>351</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G21" t="s">
         <v>423</v>
@@ -30150,7 +30201,7 @@
         <v>351</v>
       </c>
       <c r="F82" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G82" t="s">
         <v>423</v>
@@ -32687,7 +32738,7 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -32945,6 +32996,20 @@
         <v>11</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>614</v>
+      </c>
+      <c r="B19" t="s">
+        <v>615</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -32952,7 +33017,7 @@
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -33406,6 +33471,38 @@
         <v>11</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>614</v>
+      </c>
+      <c r="B15" t="s">
+        <v>615</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>834</v>
+      </c>
+      <c r="E15" t="s">
+        <v>835</v>
+      </c>
+      <c r="F15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" t="s">
+        <v>836</v>
+      </c>
+      <c r="H15" t="s">
+        <v>837</v>
+      </c>
+      <c r="I15" t="s">
+        <v>838</v>
+      </c>
+      <c r="J15" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -33413,7 +33510,7 @@
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -33671,6 +33768,20 @@
         <v>841</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>614</v>
+      </c>
+      <c r="B19" t="s">
+        <v>615</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>840</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -33678,7 +33789,7 @@
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -33984,6 +34095,26 @@
         <v>11</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>614</v>
+      </c>
+      <c r="B16" t="s">
+        <v>615</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" t="s">
+        <v>519</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -33991,7 +34122,7 @@
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -34895,6 +35026,59 @@
         <v>11</v>
       </c>
       <c r="Q17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>614</v>
+      </c>
+      <c r="B18" t="s">
+        <v>615</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>873</v>
+      </c>
+      <c r="E18" t="s">
+        <v>874</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" t="s">
+        <v>11</v>
+      </c>
+      <c r="L18" t="s">
+        <v>11</v>
+      </c>
+      <c r="M18" t="s">
+        <v>11</v>
+      </c>
+      <c r="N18" t="s">
+        <v>11</v>
+      </c>
+      <c r="O18" t="s">
+        <v>11</v>
+      </c>
+      <c r="P18" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q18" t="s">
         <v>11</v>
       </c>
     </row>
@@ -36199,7 +36383,7 @@
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -37570,6 +37754,44 @@
         <v>1019</v>
       </c>
       <c r="L36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>614</v>
+      </c>
+      <c r="B37" t="s">
+        <v>615</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>625</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1016</v>
+      </c>
+      <c r="F37" t="s">
+        <v>771</v>
+      </c>
+      <c r="G37" t="s">
+        <v>1020</v>
+      </c>
+      <c r="H37" t="s">
+        <v>1018</v>
+      </c>
+      <c r="I37" t="s">
+        <v>7</v>
+      </c>
+      <c r="J37" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" t="s">
+        <v>1019</v>
+      </c>
+      <c r="L37" t="s">
         <v>11</v>
       </c>
     </row>
@@ -41397,7 +41619,7 @@
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -41848,6 +42070,20 @@
         <v>7</v>
       </c>
       <c r="D32" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>614</v>
+      </c>
+      <c r="B33" t="s">
+        <v>615</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
         <v>625</v>
       </c>
     </row>
@@ -42550,7 +42786,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -43449,6 +43685,20 @@
         <v>7</v>
       </c>
       <c r="D64" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>614</v>
+      </c>
+      <c r="B65" t="s">
+        <v>615</v>
+      </c>
+      <c r="C65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" t="s">
         <v>625</v>
       </c>
     </row>

</xml_diff>